<commit_message>
Changes in TestCases structure. Added pre conditions column with data.
</commit_message>
<xml_diff>
--- a/Documents/Test Cases.xlsx
+++ b/Documents/Test Cases.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="122" uniqueCount="89">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="146" uniqueCount="93">
   <si>
     <t>Test Case ID</t>
   </si>
@@ -348,6 +348,20 @@
   <si>
     <t>Wyświetla się okno z podsumowaniem wyniku gracza
 zawierające sumę zdobytych punktów</t>
+  </si>
+  <si>
+    <t>Pre Conditions</t>
+  </si>
+  <si>
+    <t>Ustawienia domyślne sterowania 
+nie zostały zmienione.</t>
+  </si>
+  <si>
+    <t>-</t>
+  </si>
+  <si>
+    <t>Poziom rozpoczęcia gry nie jest 
+ostanim poziomem gry</t>
   </si>
 </sst>
 </file>
@@ -745,22 +759,22 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:G38"/>
+  <dimension ref="A1:H38"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="K1" sqref="K1"/>
+    <sheetView tabSelected="1" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
+      <selection activeCell="M5" sqref="M5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="2" max="2" width="43" customWidth="1"/>
-    <col min="3" max="3" width="43.7109375" customWidth="1"/>
-    <col min="4" max="4" width="19.5703125" customWidth="1"/>
-    <col min="5" max="5" width="50.5703125" customWidth="1"/>
-    <col min="6" max="6" width="16.140625" customWidth="1"/>
+    <col min="2" max="3" width="43" customWidth="1"/>
+    <col min="4" max="4" width="43.7109375" customWidth="1"/>
+    <col min="5" max="5" width="19.5703125" customWidth="1"/>
+    <col min="6" max="6" width="50.5703125" customWidth="1"/>
+    <col min="7" max="7" width="16.140625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" ht="51" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:8" ht="51" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A1" s="3" t="s">
         <v>0</v>
       </c>
@@ -768,522 +782,601 @@
         <v>1</v>
       </c>
       <c r="C1" s="3" t="s">
+        <v>89</v>
+      </c>
+      <c r="D1" s="3" t="s">
         <v>2</v>
       </c>
-      <c r="D1" s="3" t="s">
+      <c r="E1" s="3" t="s">
         <v>3</v>
       </c>
-      <c r="E1" s="3" t="s">
+      <c r="F1" s="3" t="s">
         <v>4</v>
       </c>
-      <c r="F1" s="3" t="s">
+      <c r="G1" s="3" t="s">
         <v>5</v>
       </c>
-      <c r="G1" s="3" t="s">
+      <c r="H1" s="3" t="s">
         <v>6</v>
       </c>
     </row>
-    <row r="2" spans="1:7" ht="105" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:8" ht="105" x14ac:dyDescent="0.25">
       <c r="A2" s="4" t="s">
         <v>7</v>
       </c>
       <c r="B2" s="4" t="s">
         <v>30</v>
       </c>
-      <c r="C2" s="5" t="s">
+      <c r="C2" s="6" t="s">
+        <v>90</v>
+      </c>
+      <c r="D2" s="5" t="s">
         <v>33</v>
       </c>
-      <c r="D2" s="4" t="s">
-        <v>31</v>
-      </c>
       <c r="E2" s="4" t="s">
+        <v>31</v>
+      </c>
+      <c r="F2" s="4" t="s">
         <v>32</v>
       </c>
-      <c r="F2" s="4"/>
       <c r="G2" s="4"/>
-    </row>
-    <row r="3" spans="1:7" ht="60" x14ac:dyDescent="0.25">
+      <c r="H2" s="4"/>
+    </row>
+    <row r="3" spans="1:8" ht="60" x14ac:dyDescent="0.25">
       <c r="A3" s="4" t="s">
         <v>8</v>
       </c>
       <c r="B3" s="4" t="s">
         <v>35</v>
       </c>
-      <c r="C3" s="5" t="s">
+      <c r="C3" s="4" t="s">
+        <v>91</v>
+      </c>
+      <c r="D3" s="5" t="s">
         <v>34</v>
       </c>
-      <c r="D3" s="4" t="s">
-        <v>31</v>
-      </c>
-      <c r="E3" s="6" t="s">
+      <c r="E3" s="4" t="s">
+        <v>31</v>
+      </c>
+      <c r="F3" s="6" t="s">
         <v>42</v>
       </c>
-      <c r="F3" s="4"/>
       <c r="G3" s="4"/>
-    </row>
-    <row r="4" spans="1:7" ht="75" x14ac:dyDescent="0.25">
+      <c r="H3" s="4"/>
+    </row>
+    <row r="4" spans="1:8" ht="75" x14ac:dyDescent="0.25">
       <c r="A4" s="4" t="s">
         <v>9</v>
       </c>
       <c r="B4" s="4" t="s">
         <v>36</v>
       </c>
-      <c r="C4" s="5" t="s">
+      <c r="C4" s="4" t="s">
+        <v>91</v>
+      </c>
+      <c r="D4" s="5" t="s">
         <v>37</v>
       </c>
-      <c r="D4" s="4" t="s">
-        <v>31</v>
-      </c>
-      <c r="E4" s="7" t="s">
+      <c r="E4" s="4" t="s">
+        <v>31</v>
+      </c>
+      <c r="F4" s="7" t="s">
         <v>41</v>
       </c>
-      <c r="F4" s="4"/>
       <c r="G4" s="4"/>
-    </row>
-    <row r="5" spans="1:7" ht="60" x14ac:dyDescent="0.25">
+      <c r="H4" s="4"/>
+    </row>
+    <row r="5" spans="1:8" ht="60" x14ac:dyDescent="0.25">
       <c r="A5" s="4" t="s">
         <v>10</v>
       </c>
       <c r="B5" s="4" t="s">
         <v>38</v>
       </c>
-      <c r="C5" s="5" t="s">
+      <c r="C5" s="4" t="s">
+        <v>91</v>
+      </c>
+      <c r="D5" s="5" t="s">
         <v>39</v>
       </c>
-      <c r="D5" s="4" t="s">
-        <v>31</v>
-      </c>
-      <c r="E5" s="6" t="s">
+      <c r="E5" s="4" t="s">
+        <v>31</v>
+      </c>
+      <c r="F5" s="6" t="s">
         <v>40</v>
       </c>
-      <c r="F5" s="4"/>
       <c r="G5" s="4"/>
-    </row>
-    <row r="6" spans="1:7" ht="75" x14ac:dyDescent="0.25">
+      <c r="H5" s="4"/>
+    </row>
+    <row r="6" spans="1:8" ht="75" x14ac:dyDescent="0.25">
       <c r="A6" s="4" t="s">
         <v>11</v>
       </c>
       <c r="B6" s="4" t="s">
         <v>43</v>
       </c>
-      <c r="C6" s="5" t="s">
+      <c r="C6" s="4" t="s">
+        <v>91</v>
+      </c>
+      <c r="D6" s="5" t="s">
         <v>85</v>
       </c>
-      <c r="D6" s="4" t="s">
-        <v>31</v>
-      </c>
-      <c r="E6" s="6" t="s">
+      <c r="E6" s="4" t="s">
+        <v>31</v>
+      </c>
+      <c r="F6" s="6" t="s">
         <v>44</v>
       </c>
-      <c r="F6" s="4"/>
       <c r="G6" s="4"/>
-    </row>
-    <row r="7" spans="1:7" ht="45" x14ac:dyDescent="0.25">
+      <c r="H6" s="4"/>
+    </row>
+    <row r="7" spans="1:8" ht="45" x14ac:dyDescent="0.25">
       <c r="A7" s="4" t="s">
         <v>12</v>
       </c>
       <c r="B7" s="4" t="s">
         <v>45</v>
       </c>
-      <c r="C7" s="5" t="s">
+      <c r="C7" s="4" t="s">
+        <v>91</v>
+      </c>
+      <c r="D7" s="5" t="s">
         <v>46</v>
       </c>
-      <c r="D7" s="4" t="s">
-        <v>31</v>
-      </c>
-      <c r="E7" s="6" t="s">
+      <c r="E7" s="4" t="s">
+        <v>31</v>
+      </c>
+      <c r="F7" s="6" t="s">
         <v>47</v>
       </c>
-      <c r="F7" s="4"/>
       <c r="G7" s="4"/>
-    </row>
-    <row r="8" spans="1:7" ht="30" x14ac:dyDescent="0.25">
+      <c r="H7" s="4"/>
+    </row>
+    <row r="8" spans="1:8" ht="30" x14ac:dyDescent="0.25">
       <c r="A8" s="4" t="s">
         <v>13</v>
       </c>
       <c r="B8" s="4" t="s">
         <v>48</v>
       </c>
-      <c r="C8" s="5" t="s">
+      <c r="C8" s="4" t="s">
+        <v>91</v>
+      </c>
+      <c r="D8" s="5" t="s">
         <v>49</v>
       </c>
-      <c r="D8" s="4" t="s">
-        <v>31</v>
-      </c>
-      <c r="E8" s="6" t="s">
+      <c r="E8" s="4" t="s">
+        <v>31</v>
+      </c>
+      <c r="F8" s="6" t="s">
         <v>50</v>
       </c>
-      <c r="F8" s="4"/>
       <c r="G8" s="4"/>
-    </row>
-    <row r="9" spans="1:7" ht="60" x14ac:dyDescent="0.25">
+      <c r="H8" s="4"/>
+    </row>
+    <row r="9" spans="1:8" ht="60" x14ac:dyDescent="0.25">
       <c r="A9" s="4" t="s">
         <v>14</v>
       </c>
       <c r="B9" s="4" t="s">
         <v>51</v>
       </c>
-      <c r="C9" s="5" t="s">
+      <c r="C9" s="4" t="s">
+        <v>91</v>
+      </c>
+      <c r="D9" s="5" t="s">
         <v>49</v>
       </c>
-      <c r="D9" s="4" t="s">
-        <v>31</v>
-      </c>
-      <c r="E9" s="6" t="s">
+      <c r="E9" s="4" t="s">
+        <v>31</v>
+      </c>
+      <c r="F9" s="6" t="s">
         <v>52</v>
       </c>
-      <c r="F9" s="4"/>
       <c r="G9" s="4"/>
-    </row>
-    <row r="10" spans="1:7" ht="60" x14ac:dyDescent="0.25">
+      <c r="H9" s="4"/>
+    </row>
+    <row r="10" spans="1:8" ht="60" x14ac:dyDescent="0.25">
       <c r="A10" s="4" t="s">
         <v>15</v>
       </c>
       <c r="B10" s="6" t="s">
         <v>55</v>
       </c>
-      <c r="C10" s="5" t="s">
+      <c r="C10" s="4" t="s">
+        <v>91</v>
+      </c>
+      <c r="D10" s="5" t="s">
         <v>53</v>
       </c>
-      <c r="D10" s="4" t="s">
-        <v>31</v>
-      </c>
-      <c r="E10" s="6" t="s">
+      <c r="E10" s="4" t="s">
+        <v>31</v>
+      </c>
+      <c r="F10" s="6" t="s">
         <v>54</v>
       </c>
-      <c r="F10" s="4"/>
       <c r="G10" s="4"/>
-    </row>
-    <row r="11" spans="1:7" ht="60" x14ac:dyDescent="0.25">
+      <c r="H10" s="4"/>
+    </row>
+    <row r="11" spans="1:8" ht="60" x14ac:dyDescent="0.25">
       <c r="A11" s="4" t="s">
         <v>16</v>
       </c>
       <c r="B11" s="4" t="s">
         <v>56</v>
       </c>
-      <c r="C11" s="5" t="s">
+      <c r="C11" s="4" t="s">
+        <v>91</v>
+      </c>
+      <c r="D11" s="5" t="s">
         <v>57</v>
       </c>
-      <c r="D11" s="4" t="s">
-        <v>31</v>
-      </c>
-      <c r="E11" s="6" t="s">
+      <c r="E11" s="4" t="s">
+        <v>31</v>
+      </c>
+      <c r="F11" s="6" t="s">
         <v>58</v>
       </c>
-      <c r="F11" s="4"/>
       <c r="G11" s="4"/>
-    </row>
-    <row r="12" spans="1:7" ht="30" x14ac:dyDescent="0.25">
+      <c r="H11" s="4"/>
+    </row>
+    <row r="12" spans="1:8" ht="30" x14ac:dyDescent="0.25">
       <c r="A12" s="4" t="s">
         <v>17</v>
       </c>
       <c r="B12" s="4" t="s">
         <v>59</v>
       </c>
-      <c r="C12" s="5" t="s">
+      <c r="C12" s="4" t="s">
+        <v>91</v>
+      </c>
+      <c r="D12" s="5" t="s">
         <v>49</v>
       </c>
-      <c r="D12" s="4" t="s">
-        <v>31</v>
-      </c>
-      <c r="E12" s="6" t="s">
+      <c r="E12" s="4" t="s">
+        <v>31</v>
+      </c>
+      <c r="F12" s="6" t="s">
         <v>60</v>
       </c>
-      <c r="F12" s="4"/>
       <c r="G12" s="4"/>
-    </row>
-    <row r="13" spans="1:7" ht="45" x14ac:dyDescent="0.25">
+      <c r="H12" s="4"/>
+    </row>
+    <row r="13" spans="1:8" ht="45" x14ac:dyDescent="0.25">
       <c r="A13" s="4" t="s">
         <v>18</v>
       </c>
       <c r="B13" s="4" t="s">
         <v>61</v>
       </c>
-      <c r="C13" s="5" t="s">
+      <c r="C13" s="4" t="s">
+        <v>91</v>
+      </c>
+      <c r="D13" s="5" t="s">
         <v>62</v>
       </c>
-      <c r="D13" s="4" t="s">
-        <v>31</v>
-      </c>
-      <c r="E13" s="6" t="s">
+      <c r="E13" s="4" t="s">
+        <v>31</v>
+      </c>
+      <c r="F13" s="6" t="s">
         <v>63</v>
       </c>
-      <c r="F13" s="4"/>
       <c r="G13" s="4"/>
-    </row>
-    <row r="14" spans="1:7" ht="60" x14ac:dyDescent="0.25">
+      <c r="H13" s="4"/>
+    </row>
+    <row r="14" spans="1:8" ht="60" x14ac:dyDescent="0.25">
       <c r="A14" s="4" t="s">
         <v>19</v>
       </c>
       <c r="B14" s="4" t="s">
         <v>64</v>
       </c>
-      <c r="C14" s="5" t="s">
+      <c r="C14" s="4" t="s">
+        <v>91</v>
+      </c>
+      <c r="D14" s="5" t="s">
         <v>65</v>
       </c>
-      <c r="D14" s="4" t="s">
-        <v>31</v>
-      </c>
-      <c r="E14" s="6" t="s">
+      <c r="E14" s="4" t="s">
+        <v>31</v>
+      </c>
+      <c r="F14" s="6" t="s">
         <v>66</v>
       </c>
-      <c r="F14" s="4"/>
       <c r="G14" s="4"/>
-    </row>
-    <row r="15" spans="1:7" ht="60" x14ac:dyDescent="0.25">
+      <c r="H14" s="4"/>
+    </row>
+    <row r="15" spans="1:8" ht="60" x14ac:dyDescent="0.25">
       <c r="A15" s="4" t="s">
         <v>20</v>
       </c>
       <c r="B15" s="6" t="s">
         <v>67</v>
       </c>
-      <c r="C15" s="5" t="s">
+      <c r="C15" s="4" t="s">
+        <v>91</v>
+      </c>
+      <c r="D15" s="5" t="s">
         <v>34</v>
       </c>
-      <c r="D15" s="4" t="s">
-        <v>31</v>
-      </c>
-      <c r="E15" s="6" t="s">
+      <c r="E15" s="4" t="s">
+        <v>31</v>
+      </c>
+      <c r="F15" s="6" t="s">
         <v>68</v>
       </c>
-      <c r="F15" s="4"/>
       <c r="G15" s="4"/>
-    </row>
-    <row r="16" spans="1:7" ht="60" x14ac:dyDescent="0.25">
+      <c r="H15" s="4"/>
+    </row>
+    <row r="16" spans="1:8" ht="60" x14ac:dyDescent="0.25">
       <c r="A16" s="4" t="s">
         <v>21</v>
       </c>
       <c r="B16" s="4" t="s">
         <v>69</v>
       </c>
-      <c r="C16" s="5" t="s">
+      <c r="C16" s="6" t="s">
+        <v>92</v>
+      </c>
+      <c r="D16" s="5" t="s">
         <v>75</v>
       </c>
-      <c r="D16" s="4" t="s">
-        <v>31</v>
-      </c>
-      <c r="E16" s="6" t="s">
+      <c r="E16" s="4" t="s">
+        <v>31</v>
+      </c>
+      <c r="F16" s="6" t="s">
         <v>70</v>
       </c>
-      <c r="F16" s="4"/>
       <c r="G16" s="4"/>
-    </row>
-    <row r="17" spans="1:7" ht="60" x14ac:dyDescent="0.25">
+      <c r="H16" s="4"/>
+    </row>
+    <row r="17" spans="1:8" ht="60" x14ac:dyDescent="0.25">
       <c r="A17" s="4" t="s">
         <v>22</v>
       </c>
       <c r="B17" s="6" t="s">
         <v>71</v>
       </c>
-      <c r="C17" s="5" t="s">
+      <c r="C17" s="4" t="s">
+        <v>91</v>
+      </c>
+      <c r="D17" s="5" t="s">
         <v>34</v>
       </c>
-      <c r="D17" s="4" t="s">
-        <v>31</v>
-      </c>
-      <c r="E17" s="6" t="s">
+      <c r="E17" s="4" t="s">
+        <v>31</v>
+      </c>
+      <c r="F17" s="6" t="s">
         <v>77</v>
       </c>
-      <c r="F17" s="4"/>
       <c r="G17" s="4"/>
-    </row>
-    <row r="18" spans="1:7" ht="75" x14ac:dyDescent="0.25">
+      <c r="H17" s="4"/>
+    </row>
+    <row r="18" spans="1:8" ht="75" x14ac:dyDescent="0.25">
       <c r="A18" s="4" t="s">
         <v>23</v>
       </c>
       <c r="B18" s="6" t="s">
         <v>72</v>
       </c>
-      <c r="C18" s="5" t="s">
+      <c r="C18" s="4" t="s">
+        <v>91</v>
+      </c>
+      <c r="D18" s="5" t="s">
         <v>37</v>
       </c>
-      <c r="D18" s="4" t="s">
-        <v>31</v>
-      </c>
-      <c r="E18" s="6" t="s">
+      <c r="E18" s="4" t="s">
+        <v>31</v>
+      </c>
+      <c r="F18" s="6" t="s">
         <v>78</v>
       </c>
-      <c r="F18" s="4"/>
       <c r="G18" s="4"/>
-    </row>
-    <row r="19" spans="1:7" ht="60" x14ac:dyDescent="0.25">
+      <c r="H18" s="4"/>
+    </row>
+    <row r="19" spans="1:8" ht="60" x14ac:dyDescent="0.25">
       <c r="A19" s="4" t="s">
         <v>24</v>
       </c>
       <c r="B19" s="6" t="s">
         <v>73</v>
       </c>
-      <c r="C19" s="5" t="s">
+      <c r="C19" s="6" t="s">
+        <v>92</v>
+      </c>
+      <c r="D19" s="5" t="s">
         <v>75</v>
       </c>
-      <c r="D19" s="4" t="s">
-        <v>31</v>
-      </c>
-      <c r="E19" s="6" t="s">
+      <c r="E19" s="4" t="s">
+        <v>31</v>
+      </c>
+      <c r="F19" s="6" t="s">
         <v>80</v>
       </c>
-      <c r="F19" s="4"/>
       <c r="G19" s="4"/>
-    </row>
-    <row r="20" spans="1:7" ht="60" x14ac:dyDescent="0.25">
+      <c r="H19" s="4"/>
+    </row>
+    <row r="20" spans="1:8" ht="60" x14ac:dyDescent="0.25">
       <c r="A20" s="4" t="s">
         <v>25</v>
       </c>
       <c r="B20" s="6" t="s">
         <v>74</v>
       </c>
-      <c r="C20" s="5" t="s">
+      <c r="C20" s="4" t="s">
+        <v>91</v>
+      </c>
+      <c r="D20" s="5" t="s">
         <v>76</v>
       </c>
-      <c r="D20" s="4" t="s">
-        <v>31</v>
-      </c>
-      <c r="E20" s="6" t="s">
+      <c r="E20" s="4" t="s">
+        <v>31</v>
+      </c>
+      <c r="F20" s="6" t="s">
         <v>79</v>
       </c>
-      <c r="F20" s="4"/>
       <c r="G20" s="4"/>
-    </row>
-    <row r="21" spans="1:7" ht="60" x14ac:dyDescent="0.25">
+      <c r="H20" s="4"/>
+    </row>
+    <row r="21" spans="1:8" ht="60" x14ac:dyDescent="0.25">
       <c r="A21" s="4" t="s">
         <v>26</v>
       </c>
       <c r="B21" s="6" t="s">
         <v>81</v>
       </c>
-      <c r="C21" s="5" t="s">
+      <c r="C21" s="4" t="s">
+        <v>91</v>
+      </c>
+      <c r="D21" s="5" t="s">
         <v>34</v>
       </c>
-      <c r="D21" s="4" t="s">
-        <v>31</v>
-      </c>
-      <c r="E21" s="6" t="s">
+      <c r="E21" s="4" t="s">
+        <v>31</v>
+      </c>
+      <c r="F21" s="6" t="s">
         <v>84</v>
       </c>
-      <c r="F21" s="4"/>
       <c r="G21" s="4"/>
-    </row>
-    <row r="22" spans="1:7" ht="60" x14ac:dyDescent="0.25">
+      <c r="H21" s="4"/>
+    </row>
+    <row r="22" spans="1:8" ht="60" x14ac:dyDescent="0.25">
       <c r="A22" s="4" t="s">
         <v>27</v>
       </c>
       <c r="B22" s="6" t="s">
         <v>82</v>
       </c>
-      <c r="C22" s="5" t="s">
+      <c r="C22" s="4" t="s">
+        <v>91</v>
+      </c>
+      <c r="D22" s="5" t="s">
         <v>39</v>
       </c>
-      <c r="D22" s="4" t="s">
-        <v>31</v>
-      </c>
-      <c r="E22" s="6" t="s">
+      <c r="E22" s="4" t="s">
+        <v>31</v>
+      </c>
+      <c r="F22" s="6" t="s">
         <v>83</v>
       </c>
-      <c r="F22" s="4"/>
       <c r="G22" s="4"/>
-    </row>
-    <row r="23" spans="1:7" ht="75" x14ac:dyDescent="0.25">
+      <c r="H22" s="4"/>
+    </row>
+    <row r="23" spans="1:8" ht="75" x14ac:dyDescent="0.25">
       <c r="A23" s="4" t="s">
         <v>28</v>
       </c>
       <c r="B23" s="6" t="s">
         <v>86</v>
       </c>
-      <c r="C23" s="5" t="s">
+      <c r="C23" s="4" t="s">
+        <v>91</v>
+      </c>
+      <c r="D23" s="5" t="s">
         <v>85</v>
       </c>
-      <c r="D23" s="4" t="s">
-        <v>31</v>
-      </c>
-      <c r="E23" s="6" t="s">
+      <c r="E23" s="4" t="s">
+        <v>31</v>
+      </c>
+      <c r="F23" s="6" t="s">
         <v>88</v>
       </c>
-      <c r="F23" s="4"/>
       <c r="G23" s="4"/>
-    </row>
-    <row r="24" spans="1:7" ht="60" x14ac:dyDescent="0.25">
+      <c r="H23" s="4"/>
+    </row>
+    <row r="24" spans="1:8" ht="60" x14ac:dyDescent="0.25">
       <c r="A24" s="4" t="s">
         <v>29</v>
       </c>
       <c r="B24" s="6" t="s">
         <v>87</v>
       </c>
-      <c r="C24" s="5" t="s">
+      <c r="C24" s="4" t="s">
+        <v>91</v>
+      </c>
+      <c r="D24" s="5" t="s">
         <v>76</v>
       </c>
-      <c r="D24" s="4" t="s">
-        <v>31</v>
-      </c>
-      <c r="E24" s="6" t="s">
+      <c r="E24" s="4" t="s">
+        <v>31</v>
+      </c>
+      <c r="F24" s="6" t="s">
         <v>88</v>
       </c>
-      <c r="F24" s="4"/>
       <c r="G24" s="4"/>
-    </row>
-    <row r="25" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="H24" s="4"/>
+    </row>
+    <row r="25" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A25" s="1"/>
       <c r="B25" s="1"/>
-      <c r="C25" s="2"/>
-      <c r="D25" s="1"/>
+      <c r="C25" s="1"/>
+      <c r="D25" s="2"/>
       <c r="E25" s="1"/>
       <c r="F25" s="1"/>
       <c r="G25" s="1"/>
-    </row>
-    <row r="26" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="H25" s="1"/>
+    </row>
+    <row r="26" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A26" s="1"/>
       <c r="B26" s="1"/>
-      <c r="C26" s="2"/>
-      <c r="D26" s="1"/>
+      <c r="C26" s="1"/>
+      <c r="D26" s="2"/>
       <c r="E26" s="1"/>
       <c r="F26" s="1"/>
       <c r="G26" s="1"/>
-    </row>
-    <row r="27" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="H26" s="1"/>
+    </row>
+    <row r="27" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A27" s="1"/>
       <c r="B27" s="1"/>
-      <c r="C27" s="2"/>
-      <c r="D27" s="1"/>
+      <c r="C27" s="1"/>
+      <c r="D27" s="2"/>
       <c r="E27" s="1"/>
       <c r="F27" s="1"/>
       <c r="G27" s="1"/>
-    </row>
-    <row r="28" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="H27" s="1"/>
+    </row>
+    <row r="28" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A28" s="1"/>
       <c r="B28" s="1"/>
-      <c r="C28" s="2"/>
-      <c r="D28" s="1"/>
+      <c r="C28" s="1"/>
+      <c r="D28" s="2"/>
       <c r="E28" s="1"/>
       <c r="F28" s="1"/>
       <c r="G28" s="1"/>
-    </row>
-    <row r="29" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="H28" s="1"/>
+    </row>
+    <row r="29" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A29" s="1"/>
       <c r="B29" s="1"/>
-      <c r="C29" s="2"/>
-      <c r="D29" s="1"/>
+      <c r="C29" s="1"/>
+      <c r="D29" s="2"/>
       <c r="E29" s="1"/>
       <c r="F29" s="1"/>
       <c r="G29" s="1"/>
-    </row>
-    <row r="30" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="H29" s="1"/>
+    </row>
+    <row r="30" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A30" s="1"/>
       <c r="B30" s="1"/>
-      <c r="C30" s="2"/>
-      <c r="D30" s="1"/>
+      <c r="C30" s="1"/>
+      <c r="D30" s="2"/>
       <c r="E30" s="1"/>
       <c r="F30" s="1"/>
       <c r="G30" s="1"/>
-    </row>
-    <row r="31" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="H30" s="1"/>
+    </row>
+    <row r="31" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A31" s="1"/>
       <c r="B31" s="1"/>
-      <c r="C31" s="2"/>
-      <c r="D31" s="1"/>
+      <c r="C31" s="1"/>
+      <c r="D31" s="2"/>
       <c r="E31" s="1"/>
       <c r="F31" s="1"/>
       <c r="G31" s="1"/>
-    </row>
-    <row r="32" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="H31" s="1"/>
+    </row>
+    <row r="32" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A32" s="1"/>
       <c r="B32" s="1"/>
       <c r="C32" s="1"/>
@@ -1291,8 +1384,9 @@
       <c r="E32" s="1"/>
       <c r="F32" s="1"/>
       <c r="G32" s="1"/>
-    </row>
-    <row r="33" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="H32" s="1"/>
+    </row>
+    <row r="33" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A33" s="1"/>
       <c r="B33" s="1"/>
       <c r="C33" s="1"/>
@@ -1300,8 +1394,9 @@
       <c r="E33" s="1"/>
       <c r="F33" s="1"/>
       <c r="G33" s="1"/>
-    </row>
-    <row r="34" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="H33" s="1"/>
+    </row>
+    <row r="34" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A34" s="1"/>
       <c r="B34" s="1"/>
       <c r="C34" s="1"/>
@@ -1309,8 +1404,9 @@
       <c r="E34" s="1"/>
       <c r="F34" s="1"/>
       <c r="G34" s="1"/>
-    </row>
-    <row r="35" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="H34" s="1"/>
+    </row>
+    <row r="35" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A35" s="1"/>
       <c r="B35" s="1"/>
       <c r="C35" s="1"/>
@@ -1318,8 +1414,9 @@
       <c r="E35" s="1"/>
       <c r="F35" s="1"/>
       <c r="G35" s="1"/>
-    </row>
-    <row r="36" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="H35" s="1"/>
+    </row>
+    <row r="36" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A36" s="1"/>
       <c r="B36" s="1"/>
       <c r="C36" s="1"/>
@@ -1327,8 +1424,9 @@
       <c r="E36" s="1"/>
       <c r="F36" s="1"/>
       <c r="G36" s="1"/>
-    </row>
-    <row r="37" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="H36" s="1"/>
+    </row>
+    <row r="37" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A37" s="1"/>
       <c r="B37" s="1"/>
       <c r="C37" s="1"/>
@@ -1336,8 +1434,9 @@
       <c r="E37" s="1"/>
       <c r="F37" s="1"/>
       <c r="G37" s="1"/>
-    </row>
-    <row r="38" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="H37" s="1"/>
+    </row>
+    <row r="38" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A38" s="1"/>
       <c r="B38" s="1"/>
       <c r="C38" s="1"/>
@@ -1345,6 +1444,7 @@
       <c r="E38" s="1"/>
       <c r="F38" s="1"/>
       <c r="G38" s="1"/>
+      <c r="H38" s="1"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
Dodanie TestCase związanych z menu gry.
</commit_message>
<xml_diff>
--- a/Documents/Test Cases.xlsx
+++ b/Documents/Test Cases.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="146" uniqueCount="93">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="188" uniqueCount="122">
   <si>
     <t>Test Case ID</t>
   </si>
@@ -362,6 +362,123 @@
   <si>
     <t>Poziom rozpoczęcia gry nie jest 
 ostanim poziomem gry</t>
+  </si>
+  <si>
+    <t>Wyświetlenie menu podczas gry</t>
+  </si>
+  <si>
+    <t>1. Uruchom aplikację
+2. Rozpocznij grę
+3. Wcisnij klawisz Esc</t>
+  </si>
+  <si>
+    <t>Wyświetla się menu gry</t>
+  </si>
+  <si>
+    <t>Wyciszenie dzwięków gry</t>
+  </si>
+  <si>
+    <t>Dźwięki w grze nie są wyciszone</t>
+  </si>
+  <si>
+    <t>1. Uruchom aplikację
+2. Rozpocznij grę
+3. Wcisnij klawisz Esc
+4. Wybierz opcję Settings w menu gry
+5. Zmień opcję "Toggle sound" klawiszem Enter
+6. Powróć do gry wciskając 2x klawisz Esc</t>
+  </si>
+  <si>
+    <t>Dźwieki w grze zostają wyciszone.</t>
+  </si>
+  <si>
+    <t>Włączenie dzwięków gry</t>
+  </si>
+  <si>
+    <t>Dźwięki w grze są wyciszone</t>
+  </si>
+  <si>
+    <t>Dźwieki w grze zostają włączone</t>
+  </si>
+  <si>
+    <t>Wybranie poziomu gry z menu</t>
+  </si>
+  <si>
+    <t>1. Uruchom aplikację
+2. Wybierz z menu opcję "Choose level"
+3. Wybierz numer poziomu</t>
+  </si>
+  <si>
+    <t>Gra rozpoczyna się od wybranego poziomu</t>
+  </si>
+  <si>
+    <t>Regulacja głośności dzwieków  w grze</t>
+  </si>
+  <si>
+    <t>1. Uruchom aplikację
+2. Rozpocznij grę
+3. Wcisnij klawisz Esc
+4. Wybierz opcję Settings w menu gry
+5. Wybierz opcję Sound Volume w menu gry
+6. Zmień poziom głośności 
+7. Powróć do gry wciskając 3x klawisz Esc</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Zmiana głosnosci dzwieków w grze odzwierciedla ustawienia </t>
+  </si>
+  <si>
+    <t>Zmiana ustawień sterowania w grze</t>
+  </si>
+  <si>
+    <t>1. Uruchom aplikację
+2. Rozpocznij grę
+3. Wcisnij klawisz Esc
+4. Wybierz opcję Settings w menu gry
+5. Wybierz opcję Controlls w menu gry
+6. Zmień ustawienia 
+    - klawisz a - ruch w lewo
+    - klawisz d - ruch w prawo
+    - klawisz s - skok
+7. Zatwierdź zmiany
+8. Powróć do gry wciskając 3x klawisz Esc</t>
+  </si>
+  <si>
+    <t>Postać porusza się w wybranym kierunku
+- klawisz a - ruch w lewo
+    - klawisz d - ruch w prawo
+    - klawisz s - skok
+Sterowanie odpowiada ustawieniom</t>
+  </si>
+  <si>
+    <t>Zamknięcie gry z poziomu menu</t>
+  </si>
+  <si>
+    <t>1. Uruchom aplikację
+2. Wybierz opcję Quit w menu gry</t>
+  </si>
+  <si>
+    <t>Gra zamyka się</t>
+  </si>
+  <si>
+    <t>TU24</t>
+  </si>
+  <si>
+    <t>TU25</t>
+  </si>
+  <si>
+    <t>TU26</t>
+  </si>
+  <si>
+    <t>TU27</t>
+  </si>
+  <si>
+    <t>TU28</t>
+  </si>
+  <si>
+    <t>TU29</t>
+  </si>
+  <si>
+    <t>TU30</t>
   </si>
 </sst>
 </file>
@@ -432,13 +549,10 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="8">
+  <cellXfs count="7">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
@@ -761,8 +875,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:H38"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <selection activeCell="M5" sqref="M5"/>
+    <sheetView tabSelected="1" topLeftCell="A24" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
+      <selection activeCell="J30" sqref="J30"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -775,606 +889,690 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:8" ht="51" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A1" s="3" t="s">
+      <c r="A1" s="2" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="3" t="s">
+      <c r="B1" s="2" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="3" t="s">
+      <c r="C1" s="2" t="s">
         <v>89</v>
       </c>
-      <c r="D1" s="3" t="s">
+      <c r="D1" s="2" t="s">
         <v>2</v>
       </c>
-      <c r="E1" s="3" t="s">
+      <c r="E1" s="2" t="s">
         <v>3</v>
       </c>
-      <c r="F1" s="3" t="s">
+      <c r="F1" s="2" t="s">
         <v>4</v>
       </c>
-      <c r="G1" s="3" t="s">
+      <c r="G1" s="2" t="s">
         <v>5</v>
       </c>
-      <c r="H1" s="3" t="s">
+      <c r="H1" s="2" t="s">
         <v>6</v>
       </c>
     </row>
     <row r="2" spans="1:8" ht="105" x14ac:dyDescent="0.25">
-      <c r="A2" s="4" t="s">
+      <c r="A2" s="3" t="s">
         <v>7</v>
       </c>
-      <c r="B2" s="4" t="s">
+      <c r="B2" s="3" t="s">
         <v>30</v>
       </c>
-      <c r="C2" s="6" t="s">
+      <c r="C2" s="5" t="s">
         <v>90</v>
       </c>
-      <c r="D2" s="5" t="s">
+      <c r="D2" s="4" t="s">
         <v>33</v>
       </c>
-      <c r="E2" s="4" t="s">
-        <v>31</v>
-      </c>
-      <c r="F2" s="4" t="s">
+      <c r="E2" s="3" t="s">
+        <v>31</v>
+      </c>
+      <c r="F2" s="3" t="s">
         <v>32</v>
       </c>
-      <c r="G2" s="4"/>
-      <c r="H2" s="4"/>
+      <c r="G2" s="3"/>
+      <c r="H2" s="3"/>
     </row>
     <row r="3" spans="1:8" ht="60" x14ac:dyDescent="0.25">
-      <c r="A3" s="4" t="s">
+      <c r="A3" s="3" t="s">
         <v>8</v>
       </c>
-      <c r="B3" s="4" t="s">
+      <c r="B3" s="3" t="s">
         <v>35</v>
       </c>
-      <c r="C3" s="4" t="s">
-        <v>91</v>
-      </c>
-      <c r="D3" s="5" t="s">
+      <c r="C3" s="3" t="s">
+        <v>91</v>
+      </c>
+      <c r="D3" s="4" t="s">
         <v>34</v>
       </c>
-      <c r="E3" s="4" t="s">
-        <v>31</v>
-      </c>
-      <c r="F3" s="6" t="s">
+      <c r="E3" s="3" t="s">
+        <v>31</v>
+      </c>
+      <c r="F3" s="5" t="s">
         <v>42</v>
       </c>
-      <c r="G3" s="4"/>
-      <c r="H3" s="4"/>
+      <c r="G3" s="3"/>
+      <c r="H3" s="3"/>
     </row>
     <row r="4" spans="1:8" ht="75" x14ac:dyDescent="0.25">
-      <c r="A4" s="4" t="s">
+      <c r="A4" s="3" t="s">
         <v>9</v>
       </c>
-      <c r="B4" s="4" t="s">
+      <c r="B4" s="3" t="s">
         <v>36</v>
       </c>
-      <c r="C4" s="4" t="s">
-        <v>91</v>
-      </c>
-      <c r="D4" s="5" t="s">
+      <c r="C4" s="3" t="s">
+        <v>91</v>
+      </c>
+      <c r="D4" s="4" t="s">
         <v>37</v>
       </c>
-      <c r="E4" s="4" t="s">
-        <v>31</v>
-      </c>
-      <c r="F4" s="7" t="s">
+      <c r="E4" s="3" t="s">
+        <v>31</v>
+      </c>
+      <c r="F4" s="6" t="s">
         <v>41</v>
       </c>
-      <c r="G4" s="4"/>
-      <c r="H4" s="4"/>
+      <c r="G4" s="3"/>
+      <c r="H4" s="3"/>
     </row>
     <row r="5" spans="1:8" ht="60" x14ac:dyDescent="0.25">
-      <c r="A5" s="4" t="s">
+      <c r="A5" s="3" t="s">
         <v>10</v>
       </c>
-      <c r="B5" s="4" t="s">
+      <c r="B5" s="3" t="s">
         <v>38</v>
       </c>
-      <c r="C5" s="4" t="s">
-        <v>91</v>
-      </c>
-      <c r="D5" s="5" t="s">
+      <c r="C5" s="3" t="s">
+        <v>91</v>
+      </c>
+      <c r="D5" s="4" t="s">
         <v>39</v>
       </c>
-      <c r="E5" s="4" t="s">
-        <v>31</v>
-      </c>
-      <c r="F5" s="6" t="s">
+      <c r="E5" s="3" t="s">
+        <v>31</v>
+      </c>
+      <c r="F5" s="5" t="s">
         <v>40</v>
       </c>
-      <c r="G5" s="4"/>
-      <c r="H5" s="4"/>
+      <c r="G5" s="3"/>
+      <c r="H5" s="3"/>
     </row>
     <row r="6" spans="1:8" ht="75" x14ac:dyDescent="0.25">
-      <c r="A6" s="4" t="s">
+      <c r="A6" s="3" t="s">
         <v>11</v>
       </c>
-      <c r="B6" s="4" t="s">
+      <c r="B6" s="3" t="s">
         <v>43</v>
       </c>
-      <c r="C6" s="4" t="s">
-        <v>91</v>
-      </c>
-      <c r="D6" s="5" t="s">
+      <c r="C6" s="3" t="s">
+        <v>91</v>
+      </c>
+      <c r="D6" s="4" t="s">
         <v>85</v>
       </c>
-      <c r="E6" s="4" t="s">
-        <v>31</v>
-      </c>
-      <c r="F6" s="6" t="s">
+      <c r="E6" s="3" t="s">
+        <v>31</v>
+      </c>
+      <c r="F6" s="5" t="s">
         <v>44</v>
       </c>
-      <c r="G6" s="4"/>
-      <c r="H6" s="4"/>
+      <c r="G6" s="3"/>
+      <c r="H6" s="3"/>
     </row>
     <row r="7" spans="1:8" ht="45" x14ac:dyDescent="0.25">
-      <c r="A7" s="4" t="s">
+      <c r="A7" s="3" t="s">
         <v>12</v>
       </c>
-      <c r="B7" s="4" t="s">
+      <c r="B7" s="3" t="s">
         <v>45</v>
       </c>
-      <c r="C7" s="4" t="s">
-        <v>91</v>
-      </c>
-      <c r="D7" s="5" t="s">
+      <c r="C7" s="3" t="s">
+        <v>91</v>
+      </c>
+      <c r="D7" s="4" t="s">
         <v>46</v>
       </c>
-      <c r="E7" s="4" t="s">
-        <v>31</v>
-      </c>
-      <c r="F7" s="6" t="s">
+      <c r="E7" s="3" t="s">
+        <v>31</v>
+      </c>
+      <c r="F7" s="5" t="s">
         <v>47</v>
       </c>
-      <c r="G7" s="4"/>
-      <c r="H7" s="4"/>
+      <c r="G7" s="3"/>
+      <c r="H7" s="3"/>
     </row>
     <row r="8" spans="1:8" ht="30" x14ac:dyDescent="0.25">
-      <c r="A8" s="4" t="s">
+      <c r="A8" s="3" t="s">
         <v>13</v>
       </c>
-      <c r="B8" s="4" t="s">
+      <c r="B8" s="3" t="s">
         <v>48</v>
       </c>
-      <c r="C8" s="4" t="s">
-        <v>91</v>
-      </c>
-      <c r="D8" s="5" t="s">
+      <c r="C8" s="3" t="s">
+        <v>91</v>
+      </c>
+      <c r="D8" s="4" t="s">
         <v>49</v>
       </c>
-      <c r="E8" s="4" t="s">
-        <v>31</v>
-      </c>
-      <c r="F8" s="6" t="s">
+      <c r="E8" s="3" t="s">
+        <v>31</v>
+      </c>
+      <c r="F8" s="5" t="s">
         <v>50</v>
       </c>
-      <c r="G8" s="4"/>
-      <c r="H8" s="4"/>
+      <c r="G8" s="3"/>
+      <c r="H8" s="3"/>
     </row>
     <row r="9" spans="1:8" ht="60" x14ac:dyDescent="0.25">
-      <c r="A9" s="4" t="s">
+      <c r="A9" s="3" t="s">
         <v>14</v>
       </c>
-      <c r="B9" s="4" t="s">
+      <c r="B9" s="3" t="s">
         <v>51</v>
       </c>
-      <c r="C9" s="4" t="s">
-        <v>91</v>
-      </c>
-      <c r="D9" s="5" t="s">
+      <c r="C9" s="3" t="s">
+        <v>91</v>
+      </c>
+      <c r="D9" s="4" t="s">
         <v>49</v>
       </c>
-      <c r="E9" s="4" t="s">
-        <v>31</v>
-      </c>
-      <c r="F9" s="6" t="s">
+      <c r="E9" s="3" t="s">
+        <v>31</v>
+      </c>
+      <c r="F9" s="5" t="s">
         <v>52</v>
       </c>
-      <c r="G9" s="4"/>
-      <c r="H9" s="4"/>
+      <c r="G9" s="3"/>
+      <c r="H9" s="3"/>
     </row>
     <row r="10" spans="1:8" ht="60" x14ac:dyDescent="0.25">
-      <c r="A10" s="4" t="s">
+      <c r="A10" s="3" t="s">
         <v>15</v>
       </c>
-      <c r="B10" s="6" t="s">
+      <c r="B10" s="5" t="s">
         <v>55</v>
       </c>
-      <c r="C10" s="4" t="s">
-        <v>91</v>
-      </c>
-      <c r="D10" s="5" t="s">
+      <c r="C10" s="3" t="s">
+        <v>91</v>
+      </c>
+      <c r="D10" s="4" t="s">
         <v>53</v>
       </c>
-      <c r="E10" s="4" t="s">
-        <v>31</v>
-      </c>
-      <c r="F10" s="6" t="s">
+      <c r="E10" s="3" t="s">
+        <v>31</v>
+      </c>
+      <c r="F10" s="5" t="s">
         <v>54</v>
       </c>
-      <c r="G10" s="4"/>
-      <c r="H10" s="4"/>
+      <c r="G10" s="3"/>
+      <c r="H10" s="3"/>
     </row>
     <row r="11" spans="1:8" ht="60" x14ac:dyDescent="0.25">
-      <c r="A11" s="4" t="s">
+      <c r="A11" s="3" t="s">
         <v>16</v>
       </c>
-      <c r="B11" s="4" t="s">
+      <c r="B11" s="3" t="s">
         <v>56</v>
       </c>
-      <c r="C11" s="4" t="s">
-        <v>91</v>
-      </c>
-      <c r="D11" s="5" t="s">
+      <c r="C11" s="3" t="s">
+        <v>91</v>
+      </c>
+      <c r="D11" s="4" t="s">
         <v>57</v>
       </c>
-      <c r="E11" s="4" t="s">
-        <v>31</v>
-      </c>
-      <c r="F11" s="6" t="s">
+      <c r="E11" s="3" t="s">
+        <v>31</v>
+      </c>
+      <c r="F11" s="5" t="s">
         <v>58</v>
       </c>
-      <c r="G11" s="4"/>
-      <c r="H11" s="4"/>
+      <c r="G11" s="3"/>
+      <c r="H11" s="3"/>
     </row>
     <row r="12" spans="1:8" ht="30" x14ac:dyDescent="0.25">
-      <c r="A12" s="4" t="s">
+      <c r="A12" s="3" t="s">
         <v>17</v>
       </c>
-      <c r="B12" s="4" t="s">
+      <c r="B12" s="3" t="s">
         <v>59</v>
       </c>
-      <c r="C12" s="4" t="s">
-        <v>91</v>
-      </c>
-      <c r="D12" s="5" t="s">
+      <c r="C12" s="3" t="s">
+        <v>91</v>
+      </c>
+      <c r="D12" s="4" t="s">
         <v>49</v>
       </c>
-      <c r="E12" s="4" t="s">
-        <v>31</v>
-      </c>
-      <c r="F12" s="6" t="s">
+      <c r="E12" s="3" t="s">
+        <v>31</v>
+      </c>
+      <c r="F12" s="5" t="s">
         <v>60</v>
       </c>
-      <c r="G12" s="4"/>
-      <c r="H12" s="4"/>
+      <c r="G12" s="3"/>
+      <c r="H12" s="3"/>
     </row>
     <row r="13" spans="1:8" ht="45" x14ac:dyDescent="0.25">
-      <c r="A13" s="4" t="s">
+      <c r="A13" s="3" t="s">
         <v>18</v>
       </c>
-      <c r="B13" s="4" t="s">
+      <c r="B13" s="3" t="s">
         <v>61</v>
       </c>
-      <c r="C13" s="4" t="s">
-        <v>91</v>
-      </c>
-      <c r="D13" s="5" t="s">
+      <c r="C13" s="3" t="s">
+        <v>91</v>
+      </c>
+      <c r="D13" s="4" t="s">
         <v>62</v>
       </c>
-      <c r="E13" s="4" t="s">
-        <v>31</v>
-      </c>
-      <c r="F13" s="6" t="s">
+      <c r="E13" s="3" t="s">
+        <v>31</v>
+      </c>
+      <c r="F13" s="5" t="s">
         <v>63</v>
       </c>
-      <c r="G13" s="4"/>
-      <c r="H13" s="4"/>
+      <c r="G13" s="3"/>
+      <c r="H13" s="3"/>
     </row>
     <row r="14" spans="1:8" ht="60" x14ac:dyDescent="0.25">
-      <c r="A14" s="4" t="s">
+      <c r="A14" s="3" t="s">
         <v>19</v>
       </c>
-      <c r="B14" s="4" t="s">
+      <c r="B14" s="3" t="s">
         <v>64</v>
       </c>
-      <c r="C14" s="4" t="s">
-        <v>91</v>
-      </c>
-      <c r="D14" s="5" t="s">
+      <c r="C14" s="3" t="s">
+        <v>91</v>
+      </c>
+      <c r="D14" s="4" t="s">
         <v>65</v>
       </c>
-      <c r="E14" s="4" t="s">
-        <v>31</v>
-      </c>
-      <c r="F14" s="6" t="s">
+      <c r="E14" s="3" t="s">
+        <v>31</v>
+      </c>
+      <c r="F14" s="5" t="s">
         <v>66</v>
       </c>
-      <c r="G14" s="4"/>
-      <c r="H14" s="4"/>
+      <c r="G14" s="3"/>
+      <c r="H14" s="3"/>
     </row>
     <row r="15" spans="1:8" ht="60" x14ac:dyDescent="0.25">
-      <c r="A15" s="4" t="s">
+      <c r="A15" s="3" t="s">
         <v>20</v>
       </c>
-      <c r="B15" s="6" t="s">
+      <c r="B15" s="5" t="s">
         <v>67</v>
       </c>
-      <c r="C15" s="4" t="s">
-        <v>91</v>
-      </c>
-      <c r="D15" s="5" t="s">
+      <c r="C15" s="3" t="s">
+        <v>91</v>
+      </c>
+      <c r="D15" s="4" t="s">
         <v>34</v>
       </c>
-      <c r="E15" s="4" t="s">
-        <v>31</v>
-      </c>
-      <c r="F15" s="6" t="s">
+      <c r="E15" s="3" t="s">
+        <v>31</v>
+      </c>
+      <c r="F15" s="5" t="s">
         <v>68</v>
       </c>
-      <c r="G15" s="4"/>
-      <c r="H15" s="4"/>
+      <c r="G15" s="3"/>
+      <c r="H15" s="3"/>
     </row>
     <row r="16" spans="1:8" ht="60" x14ac:dyDescent="0.25">
-      <c r="A16" s="4" t="s">
+      <c r="A16" s="3" t="s">
         <v>21</v>
       </c>
-      <c r="B16" s="4" t="s">
+      <c r="B16" s="3" t="s">
         <v>69</v>
       </c>
-      <c r="C16" s="6" t="s">
+      <c r="C16" s="5" t="s">
         <v>92</v>
       </c>
-      <c r="D16" s="5" t="s">
+      <c r="D16" s="4" t="s">
         <v>75</v>
       </c>
-      <c r="E16" s="4" t="s">
-        <v>31</v>
-      </c>
-      <c r="F16" s="6" t="s">
+      <c r="E16" s="3" t="s">
+        <v>31</v>
+      </c>
+      <c r="F16" s="5" t="s">
         <v>70</v>
       </c>
-      <c r="G16" s="4"/>
-      <c r="H16" s="4"/>
+      <c r="G16" s="3"/>
+      <c r="H16" s="3"/>
     </row>
     <row r="17" spans="1:8" ht="60" x14ac:dyDescent="0.25">
-      <c r="A17" s="4" t="s">
+      <c r="A17" s="3" t="s">
         <v>22</v>
       </c>
-      <c r="B17" s="6" t="s">
+      <c r="B17" s="5" t="s">
         <v>71</v>
       </c>
-      <c r="C17" s="4" t="s">
-        <v>91</v>
-      </c>
-      <c r="D17" s="5" t="s">
+      <c r="C17" s="3" t="s">
+        <v>91</v>
+      </c>
+      <c r="D17" s="4" t="s">
         <v>34</v>
       </c>
-      <c r="E17" s="4" t="s">
-        <v>31</v>
-      </c>
-      <c r="F17" s="6" t="s">
+      <c r="E17" s="3" t="s">
+        <v>31</v>
+      </c>
+      <c r="F17" s="5" t="s">
         <v>77</v>
       </c>
-      <c r="G17" s="4"/>
-      <c r="H17" s="4"/>
+      <c r="G17" s="3"/>
+      <c r="H17" s="3"/>
     </row>
     <row r="18" spans="1:8" ht="75" x14ac:dyDescent="0.25">
-      <c r="A18" s="4" t="s">
+      <c r="A18" s="3" t="s">
         <v>23</v>
       </c>
-      <c r="B18" s="6" t="s">
+      <c r="B18" s="5" t="s">
         <v>72</v>
       </c>
-      <c r="C18" s="4" t="s">
-        <v>91</v>
-      </c>
-      <c r="D18" s="5" t="s">
+      <c r="C18" s="3" t="s">
+        <v>91</v>
+      </c>
+      <c r="D18" s="4" t="s">
         <v>37</v>
       </c>
-      <c r="E18" s="4" t="s">
-        <v>31</v>
-      </c>
-      <c r="F18" s="6" t="s">
+      <c r="E18" s="3" t="s">
+        <v>31</v>
+      </c>
+      <c r="F18" s="5" t="s">
         <v>78</v>
       </c>
-      <c r="G18" s="4"/>
-      <c r="H18" s="4"/>
+      <c r="G18" s="3"/>
+      <c r="H18" s="3"/>
     </row>
     <row r="19" spans="1:8" ht="60" x14ac:dyDescent="0.25">
-      <c r="A19" s="4" t="s">
+      <c r="A19" s="3" t="s">
         <v>24</v>
       </c>
-      <c r="B19" s="6" t="s">
+      <c r="B19" s="5" t="s">
         <v>73</v>
       </c>
-      <c r="C19" s="6" t="s">
+      <c r="C19" s="5" t="s">
         <v>92</v>
       </c>
-      <c r="D19" s="5" t="s">
+      <c r="D19" s="4" t="s">
         <v>75</v>
       </c>
-      <c r="E19" s="4" t="s">
-        <v>31</v>
-      </c>
-      <c r="F19" s="6" t="s">
+      <c r="E19" s="3" t="s">
+        <v>31</v>
+      </c>
+      <c r="F19" s="5" t="s">
         <v>80</v>
       </c>
-      <c r="G19" s="4"/>
-      <c r="H19" s="4"/>
+      <c r="G19" s="3"/>
+      <c r="H19" s="3"/>
     </row>
     <row r="20" spans="1:8" ht="60" x14ac:dyDescent="0.25">
-      <c r="A20" s="4" t="s">
+      <c r="A20" s="3" t="s">
         <v>25</v>
       </c>
-      <c r="B20" s="6" t="s">
+      <c r="B20" s="5" t="s">
         <v>74</v>
       </c>
-      <c r="C20" s="4" t="s">
-        <v>91</v>
-      </c>
-      <c r="D20" s="5" t="s">
+      <c r="C20" s="3" t="s">
+        <v>91</v>
+      </c>
+      <c r="D20" s="4" t="s">
         <v>76</v>
       </c>
-      <c r="E20" s="4" t="s">
-        <v>31</v>
-      </c>
-      <c r="F20" s="6" t="s">
+      <c r="E20" s="3" t="s">
+        <v>31</v>
+      </c>
+      <c r="F20" s="5" t="s">
         <v>79</v>
       </c>
-      <c r="G20" s="4"/>
-      <c r="H20" s="4"/>
+      <c r="G20" s="3"/>
+      <c r="H20" s="3"/>
     </row>
     <row r="21" spans="1:8" ht="60" x14ac:dyDescent="0.25">
-      <c r="A21" s="4" t="s">
+      <c r="A21" s="3" t="s">
         <v>26</v>
       </c>
-      <c r="B21" s="6" t="s">
+      <c r="B21" s="5" t="s">
         <v>81</v>
       </c>
-      <c r="C21" s="4" t="s">
-        <v>91</v>
-      </c>
-      <c r="D21" s="5" t="s">
+      <c r="C21" s="3" t="s">
+        <v>91</v>
+      </c>
+      <c r="D21" s="4" t="s">
         <v>34</v>
       </c>
-      <c r="E21" s="4" t="s">
-        <v>31</v>
-      </c>
-      <c r="F21" s="6" t="s">
+      <c r="E21" s="3" t="s">
+        <v>31</v>
+      </c>
+      <c r="F21" s="5" t="s">
         <v>84</v>
       </c>
-      <c r="G21" s="4"/>
-      <c r="H21" s="4"/>
+      <c r="G21" s="3"/>
+      <c r="H21" s="3"/>
     </row>
     <row r="22" spans="1:8" ht="60" x14ac:dyDescent="0.25">
-      <c r="A22" s="4" t="s">
+      <c r="A22" s="3" t="s">
         <v>27</v>
       </c>
-      <c r="B22" s="6" t="s">
+      <c r="B22" s="5" t="s">
         <v>82</v>
       </c>
-      <c r="C22" s="4" t="s">
-        <v>91</v>
-      </c>
-      <c r="D22" s="5" t="s">
+      <c r="C22" s="3" t="s">
+        <v>91</v>
+      </c>
+      <c r="D22" s="4" t="s">
         <v>39</v>
       </c>
-      <c r="E22" s="4" t="s">
-        <v>31</v>
-      </c>
-      <c r="F22" s="6" t="s">
+      <c r="E22" s="3" t="s">
+        <v>31</v>
+      </c>
+      <c r="F22" s="5" t="s">
         <v>83</v>
       </c>
-      <c r="G22" s="4"/>
-      <c r="H22" s="4"/>
+      <c r="G22" s="3"/>
+      <c r="H22" s="3"/>
     </row>
     <row r="23" spans="1:8" ht="75" x14ac:dyDescent="0.25">
-      <c r="A23" s="4" t="s">
+      <c r="A23" s="3" t="s">
         <v>28</v>
       </c>
-      <c r="B23" s="6" t="s">
+      <c r="B23" s="5" t="s">
         <v>86</v>
       </c>
-      <c r="C23" s="4" t="s">
-        <v>91</v>
-      </c>
-      <c r="D23" s="5" t="s">
+      <c r="C23" s="3" t="s">
+        <v>91</v>
+      </c>
+      <c r="D23" s="4" t="s">
         <v>85</v>
       </c>
-      <c r="E23" s="4" t="s">
-        <v>31</v>
-      </c>
-      <c r="F23" s="6" t="s">
+      <c r="E23" s="3" t="s">
+        <v>31</v>
+      </c>
+      <c r="F23" s="5" t="s">
         <v>88</v>
       </c>
-      <c r="G23" s="4"/>
-      <c r="H23" s="4"/>
+      <c r="G23" s="3"/>
+      <c r="H23" s="3"/>
     </row>
     <row r="24" spans="1:8" ht="60" x14ac:dyDescent="0.25">
-      <c r="A24" s="4" t="s">
+      <c r="A24" s="3" t="s">
         <v>29</v>
       </c>
-      <c r="B24" s="6" t="s">
+      <c r="B24" s="5" t="s">
         <v>87</v>
       </c>
-      <c r="C24" s="4" t="s">
-        <v>91</v>
-      </c>
-      <c r="D24" s="5" t="s">
+      <c r="C24" s="3" t="s">
+        <v>91</v>
+      </c>
+      <c r="D24" s="4" t="s">
         <v>76</v>
       </c>
-      <c r="E24" s="4" t="s">
-        <v>31</v>
-      </c>
-      <c r="F24" s="6" t="s">
+      <c r="E24" s="3" t="s">
+        <v>31</v>
+      </c>
+      <c r="F24" s="5" t="s">
         <v>88</v>
       </c>
-      <c r="G24" s="4"/>
-      <c r="H24" s="4"/>
-    </row>
-    <row r="25" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A25" s="1"/>
-      <c r="B25" s="1"/>
-      <c r="C25" s="1"/>
-      <c r="D25" s="2"/>
-      <c r="E25" s="1"/>
-      <c r="F25" s="1"/>
-      <c r="G25" s="1"/>
-      <c r="H25" s="1"/>
-    </row>
-    <row r="26" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A26" s="1"/>
-      <c r="B26" s="1"/>
-      <c r="C26" s="1"/>
-      <c r="D26" s="2"/>
-      <c r="E26" s="1"/>
-      <c r="F26" s="1"/>
-      <c r="G26" s="1"/>
-      <c r="H26" s="1"/>
-    </row>
-    <row r="27" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A27" s="1"/>
-      <c r="B27" s="1"/>
-      <c r="C27" s="1"/>
-      <c r="D27" s="2"/>
-      <c r="E27" s="1"/>
-      <c r="F27" s="1"/>
-      <c r="G27" s="1"/>
-      <c r="H27" s="1"/>
-    </row>
-    <row r="28" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A28" s="1"/>
-      <c r="B28" s="1"/>
-      <c r="C28" s="1"/>
-      <c r="D28" s="2"/>
-      <c r="E28" s="1"/>
-      <c r="F28" s="1"/>
-      <c r="G28" s="1"/>
-      <c r="H28" s="1"/>
-    </row>
-    <row r="29" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A29" s="1"/>
-      <c r="B29" s="1"/>
-      <c r="C29" s="1"/>
-      <c r="D29" s="2"/>
-      <c r="E29" s="1"/>
-      <c r="F29" s="1"/>
-      <c r="G29" s="1"/>
-      <c r="H29" s="1"/>
-    </row>
-    <row r="30" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A30" s="1"/>
-      <c r="B30" s="1"/>
-      <c r="C30" s="1"/>
-      <c r="D30" s="2"/>
-      <c r="E30" s="1"/>
-      <c r="F30" s="1"/>
-      <c r="G30" s="1"/>
-      <c r="H30" s="1"/>
-    </row>
-    <row r="31" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A31" s="1"/>
-      <c r="B31" s="1"/>
-      <c r="C31" s="1"/>
-      <c r="D31" s="2"/>
-      <c r="E31" s="1"/>
-      <c r="F31" s="1"/>
-      <c r="G31" s="1"/>
-      <c r="H31" s="1"/>
+      <c r="G24" s="3"/>
+      <c r="H24" s="3"/>
+    </row>
+    <row r="25" spans="1:8" ht="45" x14ac:dyDescent="0.25">
+      <c r="A25" s="3" t="s">
+        <v>115</v>
+      </c>
+      <c r="B25" s="5" t="s">
+        <v>93</v>
+      </c>
+      <c r="C25" s="3" t="s">
+        <v>91</v>
+      </c>
+      <c r="D25" s="4" t="s">
+        <v>94</v>
+      </c>
+      <c r="E25" s="3" t="s">
+        <v>91</v>
+      </c>
+      <c r="F25" s="5" t="s">
+        <v>95</v>
+      </c>
+      <c r="G25" s="3"/>
+      <c r="H25" s="3"/>
+    </row>
+    <row r="26" spans="1:8" ht="90" x14ac:dyDescent="0.25">
+      <c r="A26" s="3" t="s">
+        <v>116</v>
+      </c>
+      <c r="B26" s="5" t="s">
+        <v>96</v>
+      </c>
+      <c r="C26" s="3" t="s">
+        <v>97</v>
+      </c>
+      <c r="D26" s="4" t="s">
+        <v>98</v>
+      </c>
+      <c r="E26" s="3" t="s">
+        <v>91</v>
+      </c>
+      <c r="F26" s="5" t="s">
+        <v>99</v>
+      </c>
+      <c r="G26" s="3"/>
+      <c r="H26" s="3"/>
+    </row>
+    <row r="27" spans="1:8" ht="90" x14ac:dyDescent="0.25">
+      <c r="A27" s="3" t="s">
+        <v>117</v>
+      </c>
+      <c r="B27" s="5" t="s">
+        <v>100</v>
+      </c>
+      <c r="C27" s="3" t="s">
+        <v>101</v>
+      </c>
+      <c r="D27" s="4" t="s">
+        <v>98</v>
+      </c>
+      <c r="E27" s="3" t="s">
+        <v>91</v>
+      </c>
+      <c r="F27" s="5" t="s">
+        <v>102</v>
+      </c>
+      <c r="G27" s="3"/>
+      <c r="H27" s="3"/>
+    </row>
+    <row r="28" spans="1:8" ht="45" x14ac:dyDescent="0.25">
+      <c r="A28" s="3" t="s">
+        <v>118</v>
+      </c>
+      <c r="B28" s="5" t="s">
+        <v>103</v>
+      </c>
+      <c r="C28" s="3" t="s">
+        <v>91</v>
+      </c>
+      <c r="D28" s="4" t="s">
+        <v>104</v>
+      </c>
+      <c r="E28" s="3" t="s">
+        <v>91</v>
+      </c>
+      <c r="F28" s="5" t="s">
+        <v>105</v>
+      </c>
+      <c r="G28" s="3"/>
+      <c r="H28" s="3"/>
+    </row>
+    <row r="29" spans="1:8" ht="105" x14ac:dyDescent="0.25">
+      <c r="A29" s="3" t="s">
+        <v>119</v>
+      </c>
+      <c r="B29" s="5" t="s">
+        <v>106</v>
+      </c>
+      <c r="C29" s="3" t="s">
+        <v>91</v>
+      </c>
+      <c r="D29" s="4" t="s">
+        <v>107</v>
+      </c>
+      <c r="E29" s="3" t="s">
+        <v>91</v>
+      </c>
+      <c r="F29" s="5" t="s">
+        <v>108</v>
+      </c>
+      <c r="G29" s="3"/>
+      <c r="H29" s="3"/>
+    </row>
+    <row r="30" spans="1:8" ht="165" x14ac:dyDescent="0.25">
+      <c r="A30" s="3" t="s">
+        <v>120</v>
+      </c>
+      <c r="B30" s="5" t="s">
+        <v>109</v>
+      </c>
+      <c r="C30" s="5" t="s">
+        <v>90</v>
+      </c>
+      <c r="D30" s="4" t="s">
+        <v>110</v>
+      </c>
+      <c r="E30" s="3" t="s">
+        <v>91</v>
+      </c>
+      <c r="F30" s="5" t="s">
+        <v>111</v>
+      </c>
+      <c r="G30" s="3"/>
+      <c r="H30" s="3"/>
+    </row>
+    <row r="31" spans="1:8" ht="30" x14ac:dyDescent="0.25">
+      <c r="A31" s="3" t="s">
+        <v>121</v>
+      </c>
+      <c r="B31" s="5" t="s">
+        <v>112</v>
+      </c>
+      <c r="C31" s="3" t="s">
+        <v>91</v>
+      </c>
+      <c r="D31" s="4" t="s">
+        <v>113</v>
+      </c>
+      <c r="E31" s="3" t="s">
+        <v>91</v>
+      </c>
+      <c r="F31" s="5" t="s">
+        <v>114</v>
+      </c>
+      <c r="G31" s="3"/>
+      <c r="H31" s="3"/>
     </row>
     <row r="32" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A32" s="1"/>

</xml_diff>

<commit_message>
Dodane wyniki testów gry.
</commit_message>
<xml_diff>
--- a/Documents/Test Cases.xlsx
+++ b/Documents/Test Cases.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="188" uniqueCount="122">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="248" uniqueCount="130">
   <si>
     <t>Test Case ID</t>
   </si>
@@ -107,9 +107,6 @@
   </si>
   <si>
     <t>Poruszanie się bohatera</t>
-  </si>
-  <si>
-    <t>n/a</t>
   </si>
   <si>
     <t>Postać porusza się w wybranym kierunku</t>
@@ -479,6 +476,37 @@
   </si>
   <si>
     <t>TU30</t>
+  </si>
+  <si>
+    <t>Pass</t>
+  </si>
+  <si>
+    <t>Wejście bohatera do zamku kończy poziom, i powoduje rozpoczęcie kolejnego poziomu,
+lub jeśli aktualny poziom jest ostatnim - koniec gry.</t>
+  </si>
+  <si>
+    <t>Bohater ma możliwość wskoczenia na równolegle położone podłoże do aktualnego na którym się znajduje. Może dokonać tego przenikając jedynie przez dolną sciankę podłoża. Boczna scianka podłoża blokuje skok.</t>
+  </si>
+  <si>
+    <t>Fail</t>
+  </si>
+  <si>
+    <t>Po uruchomieniu gry, 
+ładują się podstawowe tekstury</t>
+  </si>
+  <si>
+    <t>Brak wyswietlanej animacji podczas smierci postaci.</t>
+  </si>
+  <si>
+    <t>Podczas interakcji bohatera z przeciwnikiem,
+nie wyswietlane są animacje. Bohater lub przeciwnik 
+znika bez animacji</t>
+  </si>
+  <si>
+    <t>Po zakończeniu poziomu dzwięk nie jest odtwarzany</t>
+  </si>
+  <si>
+    <t>Wybranie opcji powoduje zamknięcie gry</t>
   </si>
 </sst>
 </file>
@@ -502,7 +530,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="4">
+  <fills count="6">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -511,13 +539,25 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FFFFFF00"/>
+        <fgColor theme="0" tint="-0.14999847407452621"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="0" tint="-0.14999847407452621"/>
+        <fgColor rgb="FF92D050"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="0"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFF0000"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -549,12 +589,12 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="7">
+  <cellXfs count="9">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
@@ -566,8 +606,14 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -875,8 +921,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:H38"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A24" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <selection activeCell="J30" sqref="J30"/>
+    <sheetView tabSelected="1" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
+      <selection activeCell="F3" sqref="F3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -885,7 +931,8 @@
     <col min="4" max="4" width="43.7109375" customWidth="1"/>
     <col min="5" max="5" width="19.5703125" customWidth="1"/>
     <col min="6" max="6" width="50.5703125" customWidth="1"/>
-    <col min="7" max="7" width="16.140625" customWidth="1"/>
+    <col min="7" max="7" width="51" customWidth="1"/>
+    <col min="8" max="8" width="25" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:8" ht="51" customHeight="1" x14ac:dyDescent="0.25">
@@ -896,7 +943,7 @@
         <v>1</v>
       </c>
       <c r="C1" s="2" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
       <c r="D1" s="2" t="s">
         <v>2</v>
@@ -922,657 +969,777 @@
         <v>30</v>
       </c>
       <c r="C2" s="5" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
       <c r="D2" s="4" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="E2" s="3" t="s">
+        <v>90</v>
+      </c>
+      <c r="F2" s="3" t="s">
         <v>31</v>
       </c>
-      <c r="F2" s="3" t="s">
-        <v>32</v>
-      </c>
-      <c r="G2" s="3"/>
-      <c r="H2" s="3"/>
-    </row>
-    <row r="3" spans="1:8" ht="60" x14ac:dyDescent="0.25">
+      <c r="G2" s="3" t="s">
+        <v>31</v>
+      </c>
+      <c r="H2" s="6" t="s">
+        <v>121</v>
+      </c>
+    </row>
+    <row r="3" spans="1:8" ht="195" x14ac:dyDescent="0.25">
       <c r="A3" s="3" t="s">
         <v>8</v>
       </c>
       <c r="B3" s="3" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="C3" s="3" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
       <c r="D3" s="4" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="E3" s="3" t="s">
-        <v>31</v>
+        <v>90</v>
       </c>
       <c r="F3" s="5" t="s">
-        <v>42</v>
-      </c>
-      <c r="G3" s="3"/>
-      <c r="H3" s="3"/>
+        <v>41</v>
+      </c>
+      <c r="G3" s="5" t="s">
+        <v>41</v>
+      </c>
+      <c r="H3" s="6" t="s">
+        <v>121</v>
+      </c>
     </row>
     <row r="4" spans="1:8" ht="75" x14ac:dyDescent="0.25">
       <c r="A4" s="3" t="s">
         <v>9</v>
       </c>
       <c r="B4" s="3" t="s">
+        <v>35</v>
+      </c>
+      <c r="C4" s="3" t="s">
+        <v>90</v>
+      </c>
+      <c r="D4" s="4" t="s">
         <v>36</v>
       </c>
-      <c r="C4" s="3" t="s">
-        <v>91</v>
-      </c>
-      <c r="D4" s="4" t="s">
-        <v>37</v>
-      </c>
       <c r="E4" s="3" t="s">
-        <v>31</v>
-      </c>
-      <c r="F4" s="6" t="s">
-        <v>41</v>
-      </c>
-      <c r="G4" s="3"/>
-      <c r="H4" s="3"/>
-    </row>
-    <row r="5" spans="1:8" ht="60" x14ac:dyDescent="0.25">
+        <v>90</v>
+      </c>
+      <c r="F4" s="7" t="s">
+        <v>40</v>
+      </c>
+      <c r="G4" s="7" t="s">
+        <v>40</v>
+      </c>
+      <c r="H4" s="6" t="s">
+        <v>121</v>
+      </c>
+    </row>
+    <row r="5" spans="1:8" ht="90" x14ac:dyDescent="0.25">
       <c r="A5" s="3" t="s">
         <v>10</v>
       </c>
       <c r="B5" s="3" t="s">
+        <v>37</v>
+      </c>
+      <c r="C5" s="3" t="s">
+        <v>90</v>
+      </c>
+      <c r="D5" s="4" t="s">
         <v>38</v>
       </c>
-      <c r="C5" s="3" t="s">
-        <v>91</v>
-      </c>
-      <c r="D5" s="4" t="s">
+      <c r="E5" s="3" t="s">
+        <v>90</v>
+      </c>
+      <c r="F5" s="5" t="s">
         <v>39</v>
       </c>
-      <c r="E5" s="3" t="s">
-        <v>31</v>
-      </c>
-      <c r="F5" s="5" t="s">
-        <v>40</v>
-      </c>
-      <c r="G5" s="3"/>
-      <c r="H5" s="3"/>
-    </row>
-    <row r="6" spans="1:8" ht="75" x14ac:dyDescent="0.25">
+      <c r="G5" s="5" t="s">
+        <v>39</v>
+      </c>
+      <c r="H5" s="6" t="s">
+        <v>121</v>
+      </c>
+    </row>
+    <row r="6" spans="1:8" ht="135" x14ac:dyDescent="0.25">
       <c r="A6" s="3" t="s">
         <v>11</v>
       </c>
       <c r="B6" s="3" t="s">
+        <v>42</v>
+      </c>
+      <c r="C6" s="3" t="s">
+        <v>90</v>
+      </c>
+      <c r="D6" s="4" t="s">
+        <v>84</v>
+      </c>
+      <c r="E6" s="3" t="s">
+        <v>90</v>
+      </c>
+      <c r="F6" s="5" t="s">
         <v>43</v>
       </c>
-      <c r="C6" s="3" t="s">
-        <v>91</v>
-      </c>
-      <c r="D6" s="4" t="s">
-        <v>85</v>
-      </c>
-      <c r="E6" s="3" t="s">
-        <v>31</v>
-      </c>
-      <c r="F6" s="5" t="s">
-        <v>44</v>
-      </c>
-      <c r="G6" s="3"/>
-      <c r="H6" s="3"/>
-    </row>
-    <row r="7" spans="1:8" ht="45" x14ac:dyDescent="0.25">
+      <c r="G6" s="5" t="s">
+        <v>43</v>
+      </c>
+      <c r="H6" s="6" t="s">
+        <v>121</v>
+      </c>
+    </row>
+    <row r="7" spans="1:8" ht="120" x14ac:dyDescent="0.25">
       <c r="A7" s="3" t="s">
         <v>12</v>
       </c>
       <c r="B7" s="3" t="s">
+        <v>44</v>
+      </c>
+      <c r="C7" s="3" t="s">
+        <v>90</v>
+      </c>
+      <c r="D7" s="4" t="s">
         <v>45</v>
       </c>
-      <c r="C7" s="3" t="s">
-        <v>91</v>
-      </c>
-      <c r="D7" s="4" t="s">
+      <c r="E7" s="3" t="s">
+        <v>90</v>
+      </c>
+      <c r="F7" s="5" t="s">
         <v>46</v>
       </c>
-      <c r="E7" s="3" t="s">
-        <v>31</v>
-      </c>
-      <c r="F7" s="5" t="s">
-        <v>47</v>
-      </c>
-      <c r="G7" s="3"/>
-      <c r="H7" s="3"/>
-    </row>
-    <row r="8" spans="1:8" ht="30" x14ac:dyDescent="0.25">
+      <c r="G7" s="5" t="s">
+        <v>46</v>
+      </c>
+      <c r="H7" s="6" t="s">
+        <v>121</v>
+      </c>
+    </row>
+    <row r="8" spans="1:8" ht="105" x14ac:dyDescent="0.25">
       <c r="A8" s="3" t="s">
         <v>13</v>
       </c>
       <c r="B8" s="3" t="s">
+        <v>47</v>
+      </c>
+      <c r="C8" s="3" t="s">
+        <v>90</v>
+      </c>
+      <c r="D8" s="4" t="s">
         <v>48</v>
       </c>
-      <c r="C8" s="3" t="s">
-        <v>91</v>
-      </c>
-      <c r="D8" s="4" t="s">
+      <c r="E8" s="3" t="s">
+        <v>90</v>
+      </c>
+      <c r="F8" s="5" t="s">
         <v>49</v>
       </c>
-      <c r="E8" s="3" t="s">
-        <v>31</v>
-      </c>
-      <c r="F8" s="5" t="s">
-        <v>50</v>
-      </c>
-      <c r="G8" s="3"/>
-      <c r="H8" s="3"/>
-    </row>
-    <row r="9" spans="1:8" ht="60" x14ac:dyDescent="0.25">
+      <c r="G8" s="5" t="s">
+        <v>49</v>
+      </c>
+      <c r="H8" s="6" t="s">
+        <v>121</v>
+      </c>
+    </row>
+    <row r="9" spans="1:8" ht="165" x14ac:dyDescent="0.25">
       <c r="A9" s="3" t="s">
         <v>14</v>
       </c>
       <c r="B9" s="3" t="s">
+        <v>50</v>
+      </c>
+      <c r="C9" s="3" t="s">
+        <v>90</v>
+      </c>
+      <c r="D9" s="4" t="s">
+        <v>48</v>
+      </c>
+      <c r="E9" s="3" t="s">
+        <v>90</v>
+      </c>
+      <c r="F9" s="5" t="s">
         <v>51</v>
       </c>
-      <c r="C9" s="3" t="s">
-        <v>91</v>
-      </c>
-      <c r="D9" s="4" t="s">
-        <v>49</v>
-      </c>
-      <c r="E9" s="3" t="s">
-        <v>31</v>
-      </c>
-      <c r="F9" s="5" t="s">
-        <v>52</v>
-      </c>
-      <c r="G9" s="3"/>
-      <c r="H9" s="3"/>
-    </row>
-    <row r="10" spans="1:8" ht="60" x14ac:dyDescent="0.25">
+      <c r="G9" s="5" t="s">
+        <v>51</v>
+      </c>
+      <c r="H9" s="6" t="s">
+        <v>121</v>
+      </c>
+    </row>
+    <row r="10" spans="1:8" ht="180" x14ac:dyDescent="0.25">
       <c r="A10" s="3" t="s">
         <v>15</v>
       </c>
       <c r="B10" s="5" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="C10" s="3" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
       <c r="D10" s="4" t="s">
+        <v>52</v>
+      </c>
+      <c r="E10" s="3" t="s">
+        <v>90</v>
+      </c>
+      <c r="F10" s="5" t="s">
         <v>53</v>
       </c>
-      <c r="E10" s="3" t="s">
-        <v>31</v>
-      </c>
-      <c r="F10" s="5" t="s">
-        <v>54</v>
-      </c>
-      <c r="G10" s="3"/>
-      <c r="H10" s="3"/>
-    </row>
-    <row r="11" spans="1:8" ht="60" x14ac:dyDescent="0.25">
+      <c r="G10" s="5" t="s">
+        <v>122</v>
+      </c>
+      <c r="H10" s="6" t="s">
+        <v>121</v>
+      </c>
+    </row>
+    <row r="11" spans="1:8" ht="240" x14ac:dyDescent="0.25">
       <c r="A11" s="3" t="s">
         <v>16</v>
       </c>
       <c r="B11" s="3" t="s">
+        <v>55</v>
+      </c>
+      <c r="C11" s="3" t="s">
+        <v>90</v>
+      </c>
+      <c r="D11" s="4" t="s">
         <v>56</v>
       </c>
-      <c r="C11" s="3" t="s">
-        <v>91</v>
-      </c>
-      <c r="D11" s="4" t="s">
+      <c r="E11" s="3" t="s">
+        <v>90</v>
+      </c>
+      <c r="F11" s="5" t="s">
         <v>57</v>
       </c>
-      <c r="E11" s="3" t="s">
-        <v>31</v>
-      </c>
-      <c r="F11" s="5" t="s">
-        <v>58</v>
-      </c>
-      <c r="G11" s="3"/>
-      <c r="H11" s="3"/>
-    </row>
-    <row r="12" spans="1:8" ht="30" x14ac:dyDescent="0.25">
+      <c r="G11" s="5" t="s">
+        <v>123</v>
+      </c>
+      <c r="H11" s="8" t="s">
+        <v>124</v>
+      </c>
+    </row>
+    <row r="12" spans="1:8" ht="90" x14ac:dyDescent="0.25">
       <c r="A12" s="3" t="s">
         <v>17</v>
       </c>
       <c r="B12" s="3" t="s">
+        <v>58</v>
+      </c>
+      <c r="C12" s="3" t="s">
+        <v>90</v>
+      </c>
+      <c r="D12" s="4" t="s">
+        <v>48</v>
+      </c>
+      <c r="E12" s="3" t="s">
+        <v>90</v>
+      </c>
+      <c r="F12" s="5" t="s">
         <v>59</v>
       </c>
-      <c r="C12" s="3" t="s">
-        <v>91</v>
-      </c>
-      <c r="D12" s="4" t="s">
-        <v>49</v>
-      </c>
-      <c r="E12" s="3" t="s">
-        <v>31</v>
-      </c>
-      <c r="F12" s="5" t="s">
-        <v>60</v>
-      </c>
-      <c r="G12" s="3"/>
-      <c r="H12" s="3"/>
-    </row>
-    <row r="13" spans="1:8" ht="45" x14ac:dyDescent="0.25">
+      <c r="G12" s="5" t="s">
+        <v>125</v>
+      </c>
+      <c r="H12" s="8" t="s">
+        <v>124</v>
+      </c>
+    </row>
+    <row r="13" spans="1:8" ht="120" x14ac:dyDescent="0.25">
       <c r="A13" s="3" t="s">
         <v>18</v>
       </c>
       <c r="B13" s="3" t="s">
+        <v>60</v>
+      </c>
+      <c r="C13" s="3" t="s">
+        <v>90</v>
+      </c>
+      <c r="D13" s="4" t="s">
         <v>61</v>
       </c>
-      <c r="C13" s="3" t="s">
-        <v>91</v>
-      </c>
-      <c r="D13" s="4" t="s">
+      <c r="E13" s="3" t="s">
+        <v>90</v>
+      </c>
+      <c r="F13" s="5" t="s">
         <v>62</v>
       </c>
-      <c r="E13" s="3" t="s">
-        <v>31</v>
-      </c>
-      <c r="F13" s="5" t="s">
-        <v>63</v>
-      </c>
-      <c r="G13" s="3"/>
-      <c r="H13" s="3"/>
+      <c r="G13" s="5" t="s">
+        <v>62</v>
+      </c>
+      <c r="H13" s="6" t="s">
+        <v>121</v>
+      </c>
     </row>
     <row r="14" spans="1:8" ht="60" x14ac:dyDescent="0.25">
       <c r="A14" s="3" t="s">
         <v>19</v>
       </c>
       <c r="B14" s="3" t="s">
+        <v>63</v>
+      </c>
+      <c r="C14" s="3" t="s">
+        <v>90</v>
+      </c>
+      <c r="D14" s="4" t="s">
         <v>64</v>
       </c>
-      <c r="C14" s="3" t="s">
-        <v>91</v>
-      </c>
-      <c r="D14" s="4" t="s">
+      <c r="E14" s="3" t="s">
+        <v>90</v>
+      </c>
+      <c r="F14" s="5" t="s">
         <v>65</v>
       </c>
-      <c r="E14" s="3" t="s">
-        <v>31</v>
-      </c>
-      <c r="F14" s="5" t="s">
-        <v>66</v>
-      </c>
-      <c r="G14" s="3"/>
-      <c r="H14" s="3"/>
-    </row>
-    <row r="15" spans="1:8" ht="60" x14ac:dyDescent="0.25">
+      <c r="G14" s="3" t="s">
+        <v>126</v>
+      </c>
+      <c r="H14" s="8" t="s">
+        <v>124</v>
+      </c>
+    </row>
+    <row r="15" spans="1:8" ht="150" x14ac:dyDescent="0.25">
       <c r="A15" s="3" t="s">
         <v>20</v>
       </c>
       <c r="B15" s="5" t="s">
+        <v>66</v>
+      </c>
+      <c r="C15" s="3" t="s">
+        <v>90</v>
+      </c>
+      <c r="D15" s="4" t="s">
+        <v>33</v>
+      </c>
+      <c r="E15" s="3" t="s">
+        <v>90</v>
+      </c>
+      <c r="F15" s="5" t="s">
         <v>67</v>
       </c>
-      <c r="C15" s="3" t="s">
-        <v>91</v>
-      </c>
-      <c r="D15" s="4" t="s">
-        <v>34</v>
-      </c>
-      <c r="E15" s="3" t="s">
-        <v>31</v>
-      </c>
-      <c r="F15" s="5" t="s">
-        <v>68</v>
-      </c>
-      <c r="G15" s="3"/>
-      <c r="H15" s="3"/>
-    </row>
-    <row r="16" spans="1:8" ht="60" x14ac:dyDescent="0.25">
+      <c r="G15" s="5" t="s">
+        <v>127</v>
+      </c>
+      <c r="H15" s="8" t="s">
+        <v>124</v>
+      </c>
+    </row>
+    <row r="16" spans="1:8" ht="105" x14ac:dyDescent="0.25">
       <c r="A16" s="3" t="s">
         <v>21</v>
       </c>
       <c r="B16" s="3" t="s">
+        <v>68</v>
+      </c>
+      <c r="C16" s="5" t="s">
+        <v>91</v>
+      </c>
+      <c r="D16" s="4" t="s">
+        <v>74</v>
+      </c>
+      <c r="E16" s="3" t="s">
+        <v>90</v>
+      </c>
+      <c r="F16" s="5" t="s">
         <v>69</v>
       </c>
-      <c r="C16" s="5" t="s">
-        <v>92</v>
-      </c>
-      <c r="D16" s="4" t="s">
-        <v>75</v>
-      </c>
-      <c r="E16" s="3" t="s">
-        <v>31</v>
-      </c>
-      <c r="F16" s="5" t="s">
-        <v>70</v>
-      </c>
-      <c r="G16" s="3"/>
-      <c r="H16" s="3"/>
-    </row>
-    <row r="17" spans="1:8" ht="60" x14ac:dyDescent="0.25">
+      <c r="G16" s="5" t="s">
+        <v>69</v>
+      </c>
+      <c r="H16" s="6" t="s">
+        <v>121</v>
+      </c>
+    </row>
+    <row r="17" spans="1:8" ht="105" x14ac:dyDescent="0.25">
       <c r="A17" s="3" t="s">
         <v>22</v>
       </c>
       <c r="B17" s="5" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="C17" s="3" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
       <c r="D17" s="4" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="E17" s="3" t="s">
-        <v>31</v>
+        <v>90</v>
       </c>
       <c r="F17" s="5" t="s">
-        <v>77</v>
-      </c>
-      <c r="G17" s="3"/>
-      <c r="H17" s="3"/>
-    </row>
-    <row r="18" spans="1:8" ht="75" x14ac:dyDescent="0.25">
+        <v>76</v>
+      </c>
+      <c r="G17" s="5" t="s">
+        <v>76</v>
+      </c>
+      <c r="H17" s="6" t="s">
+        <v>121</v>
+      </c>
+    </row>
+    <row r="18" spans="1:8" ht="90" x14ac:dyDescent="0.25">
       <c r="A18" s="3" t="s">
         <v>23</v>
       </c>
       <c r="B18" s="5" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="C18" s="3" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
       <c r="D18" s="4" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="E18" s="3" t="s">
-        <v>31</v>
+        <v>90</v>
       </c>
       <c r="F18" s="5" t="s">
-        <v>78</v>
-      </c>
-      <c r="G18" s="3"/>
-      <c r="H18" s="3"/>
+        <v>77</v>
+      </c>
+      <c r="G18" s="5" t="s">
+        <v>77</v>
+      </c>
+      <c r="H18" s="6" t="s">
+        <v>121</v>
+      </c>
     </row>
     <row r="19" spans="1:8" ht="60" x14ac:dyDescent="0.25">
       <c r="A19" s="3" t="s">
         <v>24</v>
       </c>
       <c r="B19" s="5" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="C19" s="5" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
       <c r="D19" s="4" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="E19" s="3" t="s">
-        <v>31</v>
+        <v>90</v>
       </c>
       <c r="F19" s="5" t="s">
-        <v>80</v>
-      </c>
-      <c r="G19" s="3"/>
-      <c r="H19" s="3"/>
-    </row>
-    <row r="20" spans="1:8" ht="60" x14ac:dyDescent="0.25">
+        <v>79</v>
+      </c>
+      <c r="G19" s="3" t="s">
+        <v>128</v>
+      </c>
+      <c r="H19" s="8" t="s">
+        <v>124</v>
+      </c>
+    </row>
+    <row r="20" spans="1:8" ht="75" x14ac:dyDescent="0.25">
       <c r="A20" s="3" t="s">
         <v>25</v>
       </c>
       <c r="B20" s="5" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="C20" s="3" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
       <c r="D20" s="4" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="E20" s="3" t="s">
-        <v>31</v>
+        <v>90</v>
       </c>
       <c r="F20" s="5" t="s">
-        <v>79</v>
-      </c>
-      <c r="G20" s="3"/>
-      <c r="H20" s="3"/>
-    </row>
-    <row r="21" spans="1:8" ht="60" x14ac:dyDescent="0.25">
+        <v>78</v>
+      </c>
+      <c r="G20" s="5" t="s">
+        <v>78</v>
+      </c>
+      <c r="H20" s="6" t="s">
+        <v>121</v>
+      </c>
+    </row>
+    <row r="21" spans="1:8" ht="90" x14ac:dyDescent="0.25">
       <c r="A21" s="3" t="s">
         <v>26</v>
       </c>
       <c r="B21" s="5" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="C21" s="3" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
       <c r="D21" s="4" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="E21" s="3" t="s">
-        <v>31</v>
+        <v>90</v>
       </c>
       <c r="F21" s="5" t="s">
-        <v>84</v>
-      </c>
-      <c r="G21" s="3"/>
-      <c r="H21" s="3"/>
-    </row>
-    <row r="22" spans="1:8" ht="60" x14ac:dyDescent="0.25">
+        <v>83</v>
+      </c>
+      <c r="G21" s="5" t="s">
+        <v>83</v>
+      </c>
+      <c r="H21" s="6" t="s">
+        <v>121</v>
+      </c>
+    </row>
+    <row r="22" spans="1:8" ht="90" x14ac:dyDescent="0.25">
       <c r="A22" s="3" t="s">
         <v>27</v>
       </c>
       <c r="B22" s="5" t="s">
+        <v>81</v>
+      </c>
+      <c r="C22" s="3" t="s">
+        <v>90</v>
+      </c>
+      <c r="D22" s="4" t="s">
+        <v>38</v>
+      </c>
+      <c r="E22" s="3" t="s">
+        <v>90</v>
+      </c>
+      <c r="F22" s="5" t="s">
         <v>82</v>
       </c>
-      <c r="C22" s="3" t="s">
-        <v>91</v>
-      </c>
-      <c r="D22" s="4" t="s">
-        <v>39</v>
-      </c>
-      <c r="E22" s="3" t="s">
-        <v>31</v>
-      </c>
-      <c r="F22" s="5" t="s">
-        <v>83</v>
-      </c>
-      <c r="G22" s="3"/>
-      <c r="H22" s="3"/>
-    </row>
-    <row r="23" spans="1:8" ht="75" x14ac:dyDescent="0.25">
+      <c r="G22" s="5" t="s">
+        <v>82</v>
+      </c>
+      <c r="H22" s="6" t="s">
+        <v>121</v>
+      </c>
+    </row>
+    <row r="23" spans="1:8" ht="105" x14ac:dyDescent="0.25">
       <c r="A23" s="3" t="s">
         <v>28</v>
       </c>
       <c r="B23" s="5" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="C23" s="3" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
       <c r="D23" s="4" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="E23" s="3" t="s">
-        <v>31</v>
+        <v>90</v>
       </c>
       <c r="F23" s="5" t="s">
-        <v>88</v>
-      </c>
-      <c r="G23" s="3"/>
-      <c r="H23" s="3"/>
-    </row>
-    <row r="24" spans="1:8" ht="60" x14ac:dyDescent="0.25">
+        <v>87</v>
+      </c>
+      <c r="G23" s="5" t="s">
+        <v>87</v>
+      </c>
+      <c r="H23" s="6" t="s">
+        <v>121</v>
+      </c>
+    </row>
+    <row r="24" spans="1:8" ht="105" x14ac:dyDescent="0.25">
       <c r="A24" s="3" t="s">
         <v>29</v>
       </c>
       <c r="B24" s="5" t="s">
+        <v>86</v>
+      </c>
+      <c r="C24" s="3" t="s">
+        <v>90</v>
+      </c>
+      <c r="D24" s="4" t="s">
+        <v>75</v>
+      </c>
+      <c r="E24" s="3" t="s">
+        <v>90</v>
+      </c>
+      <c r="F24" s="5" t="s">
         <v>87</v>
       </c>
-      <c r="C24" s="3" t="s">
-        <v>91</v>
-      </c>
-      <c r="D24" s="4" t="s">
-        <v>76</v>
-      </c>
-      <c r="E24" s="3" t="s">
-        <v>31</v>
-      </c>
-      <c r="F24" s="5" t="s">
-        <v>88</v>
-      </c>
-      <c r="G24" s="3"/>
-      <c r="H24" s="3"/>
+      <c r="G24" s="5" t="s">
+        <v>87</v>
+      </c>
+      <c r="H24" s="6" t="s">
+        <v>121</v>
+      </c>
     </row>
     <row r="25" spans="1:8" ht="45" x14ac:dyDescent="0.25">
       <c r="A25" s="3" t="s">
-        <v>115</v>
+        <v>114</v>
       </c>
       <c r="B25" s="5" t="s">
+        <v>92</v>
+      </c>
+      <c r="C25" s="3" t="s">
+        <v>90</v>
+      </c>
+      <c r="D25" s="4" t="s">
         <v>93</v>
       </c>
-      <c r="C25" s="3" t="s">
-        <v>91</v>
-      </c>
-      <c r="D25" s="4" t="s">
+      <c r="E25" s="3" t="s">
+        <v>90</v>
+      </c>
+      <c r="F25" s="5" t="s">
         <v>94</v>
       </c>
-      <c r="E25" s="3" t="s">
-        <v>91</v>
-      </c>
-      <c r="F25" s="5" t="s">
-        <v>95</v>
-      </c>
-      <c r="G25" s="3"/>
-      <c r="H25" s="3"/>
+      <c r="G25" s="5" t="s">
+        <v>94</v>
+      </c>
+      <c r="H25" s="6" t="s">
+        <v>121</v>
+      </c>
     </row>
     <row r="26" spans="1:8" ht="90" x14ac:dyDescent="0.25">
       <c r="A26" s="3" t="s">
-        <v>116</v>
+        <v>115</v>
       </c>
       <c r="B26" s="5" t="s">
+        <v>95</v>
+      </c>
+      <c r="C26" s="3" t="s">
         <v>96</v>
       </c>
-      <c r="C26" s="3" t="s">
+      <c r="D26" s="4" t="s">
         <v>97</v>
       </c>
-      <c r="D26" s="4" t="s">
+      <c r="E26" s="3" t="s">
+        <v>90</v>
+      </c>
+      <c r="F26" s="5" t="s">
         <v>98</v>
       </c>
-      <c r="E26" s="3" t="s">
-        <v>91</v>
-      </c>
-      <c r="F26" s="5" t="s">
-        <v>99</v>
-      </c>
-      <c r="G26" s="3"/>
-      <c r="H26" s="3"/>
+      <c r="G26" s="5" t="s">
+        <v>98</v>
+      </c>
+      <c r="H26" s="6" t="s">
+        <v>121</v>
+      </c>
     </row>
     <row r="27" spans="1:8" ht="90" x14ac:dyDescent="0.25">
       <c r="A27" s="3" t="s">
-        <v>117</v>
+        <v>116</v>
       </c>
       <c r="B27" s="5" t="s">
+        <v>99</v>
+      </c>
+      <c r="C27" s="3" t="s">
         <v>100</v>
       </c>
-      <c r="C27" s="3" t="s">
+      <c r="D27" s="4" t="s">
+        <v>97</v>
+      </c>
+      <c r="E27" s="3" t="s">
+        <v>90</v>
+      </c>
+      <c r="F27" s="5" t="s">
         <v>101</v>
       </c>
-      <c r="D27" s="4" t="s">
-        <v>98</v>
-      </c>
-      <c r="E27" s="3" t="s">
-        <v>91</v>
-      </c>
-      <c r="F27" s="5" t="s">
-        <v>102</v>
-      </c>
-      <c r="G27" s="3"/>
-      <c r="H27" s="3"/>
+      <c r="G27" s="5" t="s">
+        <v>101</v>
+      </c>
+      <c r="H27" s="6" t="s">
+        <v>121</v>
+      </c>
     </row>
     <row r="28" spans="1:8" ht="45" x14ac:dyDescent="0.25">
       <c r="A28" s="3" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
       <c r="B28" s="5" t="s">
+        <v>102</v>
+      </c>
+      <c r="C28" s="3" t="s">
+        <v>90</v>
+      </c>
+      <c r="D28" s="4" t="s">
         <v>103</v>
       </c>
-      <c r="C28" s="3" t="s">
-        <v>91</v>
-      </c>
-      <c r="D28" s="4" t="s">
+      <c r="E28" s="3" t="s">
+        <v>90</v>
+      </c>
+      <c r="F28" s="5" t="s">
         <v>104</v>
       </c>
-      <c r="E28" s="3" t="s">
-        <v>91</v>
-      </c>
-      <c r="F28" s="5" t="s">
-        <v>105</v>
-      </c>
-      <c r="G28" s="3"/>
-      <c r="H28" s="3"/>
+      <c r="G28" s="5" t="s">
+        <v>129</v>
+      </c>
+      <c r="H28" s="8" t="s">
+        <v>124</v>
+      </c>
     </row>
     <row r="29" spans="1:8" ht="105" x14ac:dyDescent="0.25">
       <c r="A29" s="3" t="s">
+        <v>118</v>
+      </c>
+      <c r="B29" s="5" t="s">
+        <v>105</v>
+      </c>
+      <c r="C29" s="3" t="s">
+        <v>90</v>
+      </c>
+      <c r="D29" s="4" t="s">
+        <v>106</v>
+      </c>
+      <c r="E29" s="3" t="s">
+        <v>90</v>
+      </c>
+      <c r="F29" s="5" t="s">
+        <v>107</v>
+      </c>
+      <c r="G29" s="5" t="s">
+        <v>107</v>
+      </c>
+      <c r="H29" s="6" t="s">
+        <v>121</v>
+      </c>
+    </row>
+    <row r="30" spans="1:8" ht="180" x14ac:dyDescent="0.25">
+      <c r="A30" s="3" t="s">
         <v>119</v>
       </c>
-      <c r="B29" s="5" t="s">
-        <v>106</v>
-      </c>
-      <c r="C29" s="3" t="s">
-        <v>91</v>
-      </c>
-      <c r="D29" s="4" t="s">
-        <v>107</v>
-      </c>
-      <c r="E29" s="3" t="s">
-        <v>91</v>
-      </c>
-      <c r="F29" s="5" t="s">
+      <c r="B30" s="5" t="s">
         <v>108</v>
       </c>
-      <c r="G29" s="3"/>
-      <c r="H29" s="3"/>
-    </row>
-    <row r="30" spans="1:8" ht="165" x14ac:dyDescent="0.25">
-      <c r="A30" s="3" t="s">
-        <v>120</v>
-      </c>
-      <c r="B30" s="5" t="s">
+      <c r="C30" s="5" t="s">
+        <v>89</v>
+      </c>
+      <c r="D30" s="4" t="s">
         <v>109</v>
       </c>
-      <c r="C30" s="5" t="s">
-        <v>90</v>
-      </c>
-      <c r="D30" s="4" t="s">
+      <c r="E30" s="3" t="s">
+        <v>90</v>
+      </c>
+      <c r="F30" s="5" t="s">
         <v>110</v>
       </c>
-      <c r="E30" s="3" t="s">
-        <v>91</v>
-      </c>
-      <c r="F30" s="5" t="s">
-        <v>111</v>
-      </c>
-      <c r="G30" s="3"/>
-      <c r="H30" s="3"/>
+      <c r="G30" s="5" t="s">
+        <v>110</v>
+      </c>
+      <c r="H30" s="6" t="s">
+        <v>121</v>
+      </c>
     </row>
     <row r="31" spans="1:8" ht="30" x14ac:dyDescent="0.25">
       <c r="A31" s="3" t="s">
-        <v>121</v>
+        <v>120</v>
       </c>
       <c r="B31" s="5" t="s">
+        <v>111</v>
+      </c>
+      <c r="C31" s="3" t="s">
+        <v>90</v>
+      </c>
+      <c r="D31" s="4" t="s">
         <v>112</v>
       </c>
-      <c r="C31" s="3" t="s">
-        <v>91</v>
-      </c>
-      <c r="D31" s="4" t="s">
+      <c r="E31" s="3" t="s">
+        <v>90</v>
+      </c>
+      <c r="F31" s="5" t="s">
         <v>113</v>
       </c>
-      <c r="E31" s="3" t="s">
-        <v>91</v>
-      </c>
-      <c r="F31" s="5" t="s">
-        <v>114</v>
-      </c>
-      <c r="G31" s="3"/>
-      <c r="H31" s="3"/>
+      <c r="G31" s="5" t="s">
+        <v>113</v>
+      </c>
+      <c r="H31" s="6" t="s">
+        <v>121</v>
+      </c>
     </row>
     <row r="32" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A32" s="1"/>

</xml_diff>

<commit_message>
Aktualizacja wyników testów dla obecnej wersji w pliku TestCases.xlsx
</commit_message>
<xml_diff>
--- a/Documents/Test Cases.xlsx
+++ b/Documents/Test Cases.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="248" uniqueCount="130">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="248" uniqueCount="129">
   <si>
     <t>Test Case ID</t>
   </si>
@@ -491,10 +491,6 @@
     <t>Fail</t>
   </si>
   <si>
-    <t>Po uruchomieniu gry, 
-ładują się podstawowe tekstury</t>
-  </si>
-  <si>
     <t>Brak wyswietlanej animacji podczas smierci postaci.</t>
   </si>
   <si>
@@ -506,7 +502,8 @@
     <t>Po zakończeniu poziomu dzwięk nie jest odtwarzany</t>
   </si>
   <si>
-    <t>Wybranie opcji powoduje zamknięcie gry</t>
+    <t>Po uruchomieniu gry, 
+ładują się tymczasowe tło</t>
   </si>
 </sst>
 </file>
@@ -921,8 +918,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:H38"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <selection activeCell="F3" sqref="F3"/>
+    <sheetView tabSelected="1" topLeftCell="A8" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
+      <selection activeCell="F17" sqref="F17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -987,7 +984,7 @@
         <v>121</v>
       </c>
     </row>
-    <row r="3" spans="1:8" ht="195" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:8" ht="60" x14ac:dyDescent="0.25">
       <c r="A3" s="3" t="s">
         <v>8</v>
       </c>
@@ -1039,7 +1036,7 @@
         <v>121</v>
       </c>
     </row>
-    <row r="5" spans="1:8" ht="90" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:8" ht="60" x14ac:dyDescent="0.25">
       <c r="A5" s="3" t="s">
         <v>10</v>
       </c>
@@ -1065,7 +1062,7 @@
         <v>121</v>
       </c>
     </row>
-    <row r="6" spans="1:8" ht="135" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:8" ht="75" x14ac:dyDescent="0.25">
       <c r="A6" s="3" t="s">
         <v>11</v>
       </c>
@@ -1091,7 +1088,7 @@
         <v>121</v>
       </c>
     </row>
-    <row r="7" spans="1:8" ht="120" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:8" ht="45" x14ac:dyDescent="0.25">
       <c r="A7" s="3" t="s">
         <v>12</v>
       </c>
@@ -1117,7 +1114,7 @@
         <v>121</v>
       </c>
     </row>
-    <row r="8" spans="1:8" ht="105" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:8" ht="30" x14ac:dyDescent="0.25">
       <c r="A8" s="3" t="s">
         <v>13</v>
       </c>
@@ -1143,7 +1140,7 @@
         <v>121</v>
       </c>
     </row>
-    <row r="9" spans="1:8" ht="165" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:8" ht="60" x14ac:dyDescent="0.25">
       <c r="A9" s="3" t="s">
         <v>14</v>
       </c>
@@ -1169,7 +1166,7 @@
         <v>121</v>
       </c>
     </row>
-    <row r="10" spans="1:8" ht="180" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:8" ht="60" x14ac:dyDescent="0.25">
       <c r="A10" s="3" t="s">
         <v>15</v>
       </c>
@@ -1195,7 +1192,7 @@
         <v>121</v>
       </c>
     </row>
-    <row r="11" spans="1:8" ht="240" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:8" ht="75" x14ac:dyDescent="0.25">
       <c r="A11" s="3" t="s">
         <v>16</v>
       </c>
@@ -1221,7 +1218,7 @@
         <v>124</v>
       </c>
     </row>
-    <row r="12" spans="1:8" ht="90" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:8" ht="30" x14ac:dyDescent="0.25">
       <c r="A12" s="3" t="s">
         <v>17</v>
       </c>
@@ -1241,13 +1238,13 @@
         <v>59</v>
       </c>
       <c r="G12" s="5" t="s">
-        <v>125</v>
+        <v>128</v>
       </c>
       <c r="H12" s="8" t="s">
         <v>124</v>
       </c>
     </row>
-    <row r="13" spans="1:8" ht="120" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:8" ht="45" x14ac:dyDescent="0.25">
       <c r="A13" s="3" t="s">
         <v>18</v>
       </c>
@@ -1293,13 +1290,13 @@
         <v>65</v>
       </c>
       <c r="G14" s="3" t="s">
-        <v>126</v>
+        <v>125</v>
       </c>
       <c r="H14" s="8" t="s">
         <v>124</v>
       </c>
     </row>
-    <row r="15" spans="1:8" ht="150" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:8" ht="60" x14ac:dyDescent="0.25">
       <c r="A15" s="3" t="s">
         <v>20</v>
       </c>
@@ -1319,13 +1316,13 @@
         <v>67</v>
       </c>
       <c r="G15" s="5" t="s">
-        <v>127</v>
+        <v>126</v>
       </c>
       <c r="H15" s="8" t="s">
         <v>124</v>
       </c>
     </row>
-    <row r="16" spans="1:8" ht="105" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:8" ht="60" x14ac:dyDescent="0.25">
       <c r="A16" s="3" t="s">
         <v>21</v>
       </c>
@@ -1351,7 +1348,7 @@
         <v>121</v>
       </c>
     </row>
-    <row r="17" spans="1:8" ht="105" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:8" ht="60" x14ac:dyDescent="0.25">
       <c r="A17" s="3" t="s">
         <v>22</v>
       </c>
@@ -1377,7 +1374,7 @@
         <v>121</v>
       </c>
     </row>
-    <row r="18" spans="1:8" ht="90" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:8" ht="75" x14ac:dyDescent="0.25">
       <c r="A18" s="3" t="s">
         <v>23</v>
       </c>
@@ -1423,13 +1420,13 @@
         <v>79</v>
       </c>
       <c r="G19" s="3" t="s">
-        <v>128</v>
+        <v>127</v>
       </c>
       <c r="H19" s="8" t="s">
         <v>124</v>
       </c>
     </row>
-    <row r="20" spans="1:8" ht="75" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:8" ht="60" x14ac:dyDescent="0.25">
       <c r="A20" s="3" t="s">
         <v>25</v>
       </c>
@@ -1455,7 +1452,7 @@
         <v>121</v>
       </c>
     </row>
-    <row r="21" spans="1:8" ht="90" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:8" ht="60" x14ac:dyDescent="0.25">
       <c r="A21" s="3" t="s">
         <v>26</v>
       </c>
@@ -1481,7 +1478,7 @@
         <v>121</v>
       </c>
     </row>
-    <row r="22" spans="1:8" ht="90" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:8" ht="60" x14ac:dyDescent="0.25">
       <c r="A22" s="3" t="s">
         <v>27</v>
       </c>
@@ -1507,7 +1504,7 @@
         <v>121</v>
       </c>
     </row>
-    <row r="23" spans="1:8" ht="105" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:8" ht="75" x14ac:dyDescent="0.25">
       <c r="A23" s="3" t="s">
         <v>28</v>
       </c>
@@ -1533,7 +1530,7 @@
         <v>121</v>
       </c>
     </row>
-    <row r="24" spans="1:8" ht="105" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:8" ht="60" x14ac:dyDescent="0.25">
       <c r="A24" s="3" t="s">
         <v>29</v>
       </c>
@@ -1657,10 +1654,10 @@
         <v>104</v>
       </c>
       <c r="G28" s="5" t="s">
-        <v>129</v>
-      </c>
-      <c r="H28" s="8" t="s">
-        <v>124</v>
+        <v>104</v>
+      </c>
+      <c r="H28" s="6" t="s">
+        <v>121</v>
       </c>
     </row>
     <row r="29" spans="1:8" ht="105" x14ac:dyDescent="0.25">
@@ -1689,7 +1686,7 @@
         <v>121</v>
       </c>
     </row>
-    <row r="30" spans="1:8" ht="180" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:8" ht="165" x14ac:dyDescent="0.25">
       <c r="A30" s="3" t="s">
         <v>119</v>
       </c>

</xml_diff>

<commit_message>
Aktualizacja wyników testów w pliku TestCases.xlsx
</commit_message>
<xml_diff>
--- a/Documents/Test Cases.xlsx
+++ b/Documents/Test Cases.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="248" uniqueCount="129">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="248" uniqueCount="128">
   <si>
     <t>Test Case ID</t>
   </si>
@@ -485,9 +485,6 @@
 lub jeśli aktualny poziom jest ostatnim - koniec gry.</t>
   </si>
   <si>
-    <t>Bohater ma możliwość wskoczenia na równolegle położone podłoże do aktualnego na którym się znajduje. Może dokonać tego przenikając jedynie przez dolną sciankę podłoża. Boczna scianka podłoża blokuje skok.</t>
-  </si>
-  <si>
     <t>Fail</t>
   </si>
   <si>
@@ -502,8 +499,8 @@
     <t>Po zakończeniu poziomu dzwięk nie jest odtwarzany</t>
   </si>
   <si>
-    <t>Po uruchomieniu gry, 
-ładują się tymczasowe tło</t>
+    <t>Bohater ma możliwość wskoczenia na równolegle położone podłoże do aktualnego na którym się znajduje. Może dokonać tego przenikając jedynie przez dolną sciankę podłoża. Boczna scianka podłoża blokuje skok.
+- Zmiana wymagań - boczna ścianka powinna blokować skok.</t>
   </si>
 </sst>
 </file>
@@ -918,8 +915,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:H38"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A8" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
-      <selection activeCell="F17" sqref="F17"/>
+    <sheetView tabSelected="1" topLeftCell="A29" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
+      <selection activeCell="H12" sqref="H12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1192,7 +1189,7 @@
         <v>121</v>
       </c>
     </row>
-    <row r="11" spans="1:8" ht="75" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:8" ht="105" x14ac:dyDescent="0.25">
       <c r="A11" s="3" t="s">
         <v>16</v>
       </c>
@@ -1212,10 +1209,10 @@
         <v>57</v>
       </c>
       <c r="G11" s="5" t="s">
-        <v>123</v>
-      </c>
-      <c r="H11" s="8" t="s">
-        <v>124</v>
+        <v>127</v>
+      </c>
+      <c r="H11" s="6" t="s">
+        <v>121</v>
       </c>
     </row>
     <row r="12" spans="1:8" ht="30" x14ac:dyDescent="0.25">
@@ -1238,10 +1235,10 @@
         <v>59</v>
       </c>
       <c r="G12" s="5" t="s">
-        <v>128</v>
-      </c>
-      <c r="H12" s="8" t="s">
-        <v>124</v>
+        <v>59</v>
+      </c>
+      <c r="H12" s="6" t="s">
+        <v>121</v>
       </c>
     </row>
     <row r="13" spans="1:8" ht="45" x14ac:dyDescent="0.25">
@@ -1290,10 +1287,10 @@
         <v>65</v>
       </c>
       <c r="G14" s="3" t="s">
-        <v>125</v>
+        <v>124</v>
       </c>
       <c r="H14" s="8" t="s">
-        <v>124</v>
+        <v>123</v>
       </c>
     </row>
     <row r="15" spans="1:8" ht="60" x14ac:dyDescent="0.25">
@@ -1316,10 +1313,10 @@
         <v>67</v>
       </c>
       <c r="G15" s="5" t="s">
-        <v>126</v>
+        <v>125</v>
       </c>
       <c r="H15" s="8" t="s">
-        <v>124</v>
+        <v>123</v>
       </c>
     </row>
     <row r="16" spans="1:8" ht="60" x14ac:dyDescent="0.25">
@@ -1420,10 +1417,10 @@
         <v>79</v>
       </c>
       <c r="G19" s="3" t="s">
-        <v>127</v>
+        <v>126</v>
       </c>
       <c r="H19" s="8" t="s">
-        <v>124</v>
+        <v>123</v>
       </c>
     </row>
     <row r="20" spans="1:8" ht="60" x14ac:dyDescent="0.25">

</xml_diff>

<commit_message>
TestCases - Last update
</commit_message>
<xml_diff>
--- a/Documents/Test Cases.xlsx
+++ b/Documents/Test Cases.xlsx
@@ -915,8 +915,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:H38"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A29" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
-      <selection activeCell="H12" sqref="H12"/>
+    <sheetView tabSelected="1" topLeftCell="B4" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
+      <selection activeCell="C6" sqref="C6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1419,8 +1419,8 @@
       <c r="G19" s="3" t="s">
         <v>126</v>
       </c>
-      <c r="H19" s="8" t="s">
-        <v>123</v>
+      <c r="H19" s="6" t="s">
+        <v>121</v>
       </c>
     </row>
     <row r="20" spans="1:8" ht="60" x14ac:dyDescent="0.25">
@@ -1807,6 +1807,6 @@
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup paperSize="9" scale="68" orientation="landscape" r:id="rId1"/>
+  <pageSetup paperSize="9" scale="47" orientation="landscape" r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
Test Cases.xlsx file update.
</commit_message>
<xml_diff>
--- a/Documents/Test Cases.xlsx
+++ b/Documents/Test Cases.xlsx
@@ -7,14 +7,17 @@
     <workbookView xWindow="240" yWindow="105" windowWidth="14805" windowHeight="8010"/>
   </bookViews>
   <sheets>
-    <sheet name="Arkusz1" sheetId="1" r:id="rId1"/>
+    <sheet name="Sprint I" sheetId="2" r:id="rId1"/>
+    <sheet name="Sprint II" sheetId="3" r:id="rId2"/>
+    <sheet name="Sprint III" sheetId="4" r:id="rId3"/>
+    <sheet name="All" sheetId="1" r:id="rId4"/>
   </sheets>
   <calcPr calcId="122211"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="248" uniqueCount="128">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="512" uniqueCount="128">
   <si>
     <t>Test Case ID</t>
   </si>
@@ -913,10 +916,946 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:H8"/>
+  <sheetViews>
+    <sheetView tabSelected="1" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
+      <selection activeCell="M6" sqref="M6"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="12" customWidth="1"/>
+    <col min="2" max="2" width="42.42578125" customWidth="1"/>
+    <col min="3" max="3" width="31.85546875" customWidth="1"/>
+    <col min="4" max="4" width="39.42578125" customWidth="1"/>
+    <col min="5" max="5" width="20.7109375" customWidth="1"/>
+    <col min="6" max="6" width="44" customWidth="1"/>
+    <col min="7" max="7" width="44.5703125" customWidth="1"/>
+    <col min="8" max="8" width="20.28515625" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:8" ht="51" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A1" s="2" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" s="2" t="s">
+        <v>88</v>
+      </c>
+      <c r="D1" s="2" t="s">
+        <v>2</v>
+      </c>
+      <c r="E1" s="2" t="s">
+        <v>3</v>
+      </c>
+      <c r="F1" s="2" t="s">
+        <v>4</v>
+      </c>
+      <c r="G1" s="2" t="s">
+        <v>5</v>
+      </c>
+      <c r="H1" s="2" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="2" spans="1:8" ht="105" x14ac:dyDescent="0.25">
+      <c r="A2" s="3" t="s">
+        <v>7</v>
+      </c>
+      <c r="B2" s="3" t="s">
+        <v>30</v>
+      </c>
+      <c r="C2" s="5" t="s">
+        <v>89</v>
+      </c>
+      <c r="D2" s="4" t="s">
+        <v>32</v>
+      </c>
+      <c r="E2" s="3" t="s">
+        <v>90</v>
+      </c>
+      <c r="F2" s="3" t="s">
+        <v>31</v>
+      </c>
+      <c r="G2" s="3" t="s">
+        <v>31</v>
+      </c>
+      <c r="H2" s="6" t="s">
+        <v>121</v>
+      </c>
+    </row>
+    <row r="3" spans="1:8" ht="60" x14ac:dyDescent="0.25">
+      <c r="A3" s="3" t="s">
+        <v>10</v>
+      </c>
+      <c r="B3" s="3" t="s">
+        <v>37</v>
+      </c>
+      <c r="C3" s="3" t="s">
+        <v>90</v>
+      </c>
+      <c r="D3" s="4" t="s">
+        <v>38</v>
+      </c>
+      <c r="E3" s="3" t="s">
+        <v>90</v>
+      </c>
+      <c r="F3" s="5" t="s">
+        <v>39</v>
+      </c>
+      <c r="G3" s="5" t="s">
+        <v>39</v>
+      </c>
+      <c r="H3" s="6" t="s">
+        <v>121</v>
+      </c>
+    </row>
+    <row r="4" spans="1:8" ht="75" x14ac:dyDescent="0.25">
+      <c r="A4" s="3" t="s">
+        <v>11</v>
+      </c>
+      <c r="B4" s="3" t="s">
+        <v>42</v>
+      </c>
+      <c r="C4" s="3" t="s">
+        <v>90</v>
+      </c>
+      <c r="D4" s="4" t="s">
+        <v>84</v>
+      </c>
+      <c r="E4" s="3" t="s">
+        <v>90</v>
+      </c>
+      <c r="F4" s="5" t="s">
+        <v>43</v>
+      </c>
+      <c r="G4" s="5" t="s">
+        <v>43</v>
+      </c>
+      <c r="H4" s="6" t="s">
+        <v>121</v>
+      </c>
+    </row>
+    <row r="5" spans="1:8" ht="30" x14ac:dyDescent="0.25">
+      <c r="A5" s="3" t="s">
+        <v>13</v>
+      </c>
+      <c r="B5" s="3" t="s">
+        <v>47</v>
+      </c>
+      <c r="C5" s="3" t="s">
+        <v>90</v>
+      </c>
+      <c r="D5" s="4" t="s">
+        <v>48</v>
+      </c>
+      <c r="E5" s="3" t="s">
+        <v>90</v>
+      </c>
+      <c r="F5" s="5" t="s">
+        <v>49</v>
+      </c>
+      <c r="G5" s="5" t="s">
+        <v>49</v>
+      </c>
+      <c r="H5" s="6" t="s">
+        <v>121</v>
+      </c>
+    </row>
+    <row r="6" spans="1:8" ht="60" x14ac:dyDescent="0.25">
+      <c r="A6" s="3" t="s">
+        <v>14</v>
+      </c>
+      <c r="B6" s="3" t="s">
+        <v>50</v>
+      </c>
+      <c r="C6" s="3" t="s">
+        <v>90</v>
+      </c>
+      <c r="D6" s="4" t="s">
+        <v>48</v>
+      </c>
+      <c r="E6" s="3" t="s">
+        <v>90</v>
+      </c>
+      <c r="F6" s="5" t="s">
+        <v>51</v>
+      </c>
+      <c r="G6" s="5" t="s">
+        <v>51</v>
+      </c>
+      <c r="H6" s="6" t="s">
+        <v>121</v>
+      </c>
+    </row>
+    <row r="7" spans="1:8" ht="105" x14ac:dyDescent="0.25">
+      <c r="A7" s="3" t="s">
+        <v>16</v>
+      </c>
+      <c r="B7" s="3" t="s">
+        <v>55</v>
+      </c>
+      <c r="C7" s="3" t="s">
+        <v>90</v>
+      </c>
+      <c r="D7" s="4" t="s">
+        <v>56</v>
+      </c>
+      <c r="E7" s="3" t="s">
+        <v>90</v>
+      </c>
+      <c r="F7" s="5" t="s">
+        <v>57</v>
+      </c>
+      <c r="G7" s="5" t="s">
+        <v>127</v>
+      </c>
+      <c r="H7" s="6" t="s">
+        <v>121</v>
+      </c>
+    </row>
+    <row r="8" spans="1:8" ht="60" x14ac:dyDescent="0.25">
+      <c r="A8" s="3" t="s">
+        <v>27</v>
+      </c>
+      <c r="B8" s="5" t="s">
+        <v>81</v>
+      </c>
+      <c r="C8" s="3" t="s">
+        <v>90</v>
+      </c>
+      <c r="D8" s="4" t="s">
+        <v>38</v>
+      </c>
+      <c r="E8" s="3" t="s">
+        <v>90</v>
+      </c>
+      <c r="F8" s="5" t="s">
+        <v>82</v>
+      </c>
+      <c r="G8" s="5" t="s">
+        <v>82</v>
+      </c>
+      <c r="H8" s="6" t="s">
+        <v>121</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" scale="52" orientation="landscape" verticalDpi="300" r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:H13"/>
+  <sheetViews>
+    <sheetView zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
+      <selection activeCell="H6" sqref="H6"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="12.85546875" customWidth="1"/>
+    <col min="2" max="2" width="47" customWidth="1"/>
+    <col min="3" max="3" width="31" customWidth="1"/>
+    <col min="4" max="4" width="49.42578125" customWidth="1"/>
+    <col min="5" max="5" width="14.28515625" customWidth="1"/>
+    <col min="6" max="6" width="39.28515625" customWidth="1"/>
+    <col min="7" max="7" width="40.85546875" customWidth="1"/>
+    <col min="8" max="8" width="24" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:8" ht="51" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A1" s="2" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" s="2" t="s">
+        <v>88</v>
+      </c>
+      <c r="D1" s="2" t="s">
+        <v>2</v>
+      </c>
+      <c r="E1" s="2" t="s">
+        <v>3</v>
+      </c>
+      <c r="F1" s="2" t="s">
+        <v>4</v>
+      </c>
+      <c r="G1" s="2" t="s">
+        <v>5</v>
+      </c>
+      <c r="H1" s="2" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="2" spans="1:8" ht="60" x14ac:dyDescent="0.25">
+      <c r="A2" s="3" t="s">
+        <v>8</v>
+      </c>
+      <c r="B2" s="3" t="s">
+        <v>34</v>
+      </c>
+      <c r="C2" s="3" t="s">
+        <v>90</v>
+      </c>
+      <c r="D2" s="4" t="s">
+        <v>33</v>
+      </c>
+      <c r="E2" s="3" t="s">
+        <v>90</v>
+      </c>
+      <c r="F2" s="5" t="s">
+        <v>41</v>
+      </c>
+      <c r="G2" s="5" t="s">
+        <v>41</v>
+      </c>
+      <c r="H2" s="6" t="s">
+        <v>121</v>
+      </c>
+    </row>
+    <row r="3" spans="1:8" ht="75" x14ac:dyDescent="0.25">
+      <c r="A3" s="3" t="s">
+        <v>9</v>
+      </c>
+      <c r="B3" s="3" t="s">
+        <v>35</v>
+      </c>
+      <c r="C3" s="3" t="s">
+        <v>90</v>
+      </c>
+      <c r="D3" s="4" t="s">
+        <v>36</v>
+      </c>
+      <c r="E3" s="3" t="s">
+        <v>90</v>
+      </c>
+      <c r="F3" s="7" t="s">
+        <v>40</v>
+      </c>
+      <c r="G3" s="7" t="s">
+        <v>40</v>
+      </c>
+      <c r="H3" s="6" t="s">
+        <v>121</v>
+      </c>
+    </row>
+    <row r="4" spans="1:8" ht="45" x14ac:dyDescent="0.25">
+      <c r="A4" s="3" t="s">
+        <v>12</v>
+      </c>
+      <c r="B4" s="3" t="s">
+        <v>44</v>
+      </c>
+      <c r="C4" s="3" t="s">
+        <v>90</v>
+      </c>
+      <c r="D4" s="4" t="s">
+        <v>45</v>
+      </c>
+      <c r="E4" s="3" t="s">
+        <v>90</v>
+      </c>
+      <c r="F4" s="5" t="s">
+        <v>46</v>
+      </c>
+      <c r="G4" s="5" t="s">
+        <v>46</v>
+      </c>
+      <c r="H4" s="6" t="s">
+        <v>121</v>
+      </c>
+    </row>
+    <row r="5" spans="1:8" ht="30" x14ac:dyDescent="0.25">
+      <c r="A5" s="3" t="s">
+        <v>17</v>
+      </c>
+      <c r="B5" s="3" t="s">
+        <v>58</v>
+      </c>
+      <c r="C5" s="3" t="s">
+        <v>90</v>
+      </c>
+      <c r="D5" s="4" t="s">
+        <v>48</v>
+      </c>
+      <c r="E5" s="3" t="s">
+        <v>90</v>
+      </c>
+      <c r="F5" s="5" t="s">
+        <v>59</v>
+      </c>
+      <c r="G5" s="5" t="s">
+        <v>59</v>
+      </c>
+      <c r="H5" s="6" t="s">
+        <v>121</v>
+      </c>
+    </row>
+    <row r="6" spans="1:8" ht="60" x14ac:dyDescent="0.25">
+      <c r="A6" s="3" t="s">
+        <v>21</v>
+      </c>
+      <c r="B6" s="3" t="s">
+        <v>68</v>
+      </c>
+      <c r="C6" s="5" t="s">
+        <v>91</v>
+      </c>
+      <c r="D6" s="4" t="s">
+        <v>74</v>
+      </c>
+      <c r="E6" s="3" t="s">
+        <v>90</v>
+      </c>
+      <c r="F6" s="5" t="s">
+        <v>69</v>
+      </c>
+      <c r="G6" s="5" t="s">
+        <v>69</v>
+      </c>
+      <c r="H6" s="6" t="s">
+        <v>121</v>
+      </c>
+    </row>
+    <row r="7" spans="1:8" ht="60" x14ac:dyDescent="0.25">
+      <c r="A7" s="3" t="s">
+        <v>22</v>
+      </c>
+      <c r="B7" s="5" t="s">
+        <v>70</v>
+      </c>
+      <c r="C7" s="3" t="s">
+        <v>90</v>
+      </c>
+      <c r="D7" s="4" t="s">
+        <v>33</v>
+      </c>
+      <c r="E7" s="3" t="s">
+        <v>90</v>
+      </c>
+      <c r="F7" s="5" t="s">
+        <v>76</v>
+      </c>
+      <c r="G7" s="5" t="s">
+        <v>76</v>
+      </c>
+      <c r="H7" s="6" t="s">
+        <v>121</v>
+      </c>
+    </row>
+    <row r="8" spans="1:8" ht="75" x14ac:dyDescent="0.25">
+      <c r="A8" s="3" t="s">
+        <v>23</v>
+      </c>
+      <c r="B8" s="5" t="s">
+        <v>71</v>
+      </c>
+      <c r="C8" s="3" t="s">
+        <v>90</v>
+      </c>
+      <c r="D8" s="4" t="s">
+        <v>36</v>
+      </c>
+      <c r="E8" s="3" t="s">
+        <v>90</v>
+      </c>
+      <c r="F8" s="5" t="s">
+        <v>77</v>
+      </c>
+      <c r="G8" s="5" t="s">
+        <v>77</v>
+      </c>
+      <c r="H8" s="6" t="s">
+        <v>121</v>
+      </c>
+    </row>
+    <row r="9" spans="1:8" ht="60" x14ac:dyDescent="0.25">
+      <c r="A9" s="3" t="s">
+        <v>26</v>
+      </c>
+      <c r="B9" s="5" t="s">
+        <v>80</v>
+      </c>
+      <c r="C9" s="3" t="s">
+        <v>90</v>
+      </c>
+      <c r="D9" s="4" t="s">
+        <v>33</v>
+      </c>
+      <c r="E9" s="3" t="s">
+        <v>90</v>
+      </c>
+      <c r="F9" s="5" t="s">
+        <v>83</v>
+      </c>
+      <c r="G9" s="5" t="s">
+        <v>83</v>
+      </c>
+      <c r="H9" s="6" t="s">
+        <v>121</v>
+      </c>
+    </row>
+    <row r="10" spans="1:8" ht="45" x14ac:dyDescent="0.25">
+      <c r="A10" s="3" t="s">
+        <v>114</v>
+      </c>
+      <c r="B10" s="5" t="s">
+        <v>92</v>
+      </c>
+      <c r="C10" s="3" t="s">
+        <v>90</v>
+      </c>
+      <c r="D10" s="4" t="s">
+        <v>93</v>
+      </c>
+      <c r="E10" s="3" t="s">
+        <v>90</v>
+      </c>
+      <c r="F10" s="5" t="s">
+        <v>94</v>
+      </c>
+      <c r="G10" s="5" t="s">
+        <v>94</v>
+      </c>
+      <c r="H10" s="6" t="s">
+        <v>121</v>
+      </c>
+    </row>
+    <row r="11" spans="1:8" ht="90" x14ac:dyDescent="0.25">
+      <c r="A11" s="3" t="s">
+        <v>115</v>
+      </c>
+      <c r="B11" s="5" t="s">
+        <v>95</v>
+      </c>
+      <c r="C11" s="3" t="s">
+        <v>96</v>
+      </c>
+      <c r="D11" s="4" t="s">
+        <v>97</v>
+      </c>
+      <c r="E11" s="3" t="s">
+        <v>90</v>
+      </c>
+      <c r="F11" s="5" t="s">
+        <v>98</v>
+      </c>
+      <c r="G11" s="5" t="s">
+        <v>98</v>
+      </c>
+      <c r="H11" s="6" t="s">
+        <v>121</v>
+      </c>
+    </row>
+    <row r="12" spans="1:8" ht="90" x14ac:dyDescent="0.25">
+      <c r="A12" s="3" t="s">
+        <v>116</v>
+      </c>
+      <c r="B12" s="5" t="s">
+        <v>99</v>
+      </c>
+      <c r="C12" s="3" t="s">
+        <v>100</v>
+      </c>
+      <c r="D12" s="4" t="s">
+        <v>97</v>
+      </c>
+      <c r="E12" s="3" t="s">
+        <v>90</v>
+      </c>
+      <c r="F12" s="5" t="s">
+        <v>101</v>
+      </c>
+      <c r="G12" s="5" t="s">
+        <v>101</v>
+      </c>
+      <c r="H12" s="6" t="s">
+        <v>121</v>
+      </c>
+    </row>
+    <row r="13" spans="1:8" ht="30" x14ac:dyDescent="0.25">
+      <c r="A13" s="3" t="s">
+        <v>120</v>
+      </c>
+      <c r="B13" s="5" t="s">
+        <v>111</v>
+      </c>
+      <c r="C13" s="3" t="s">
+        <v>90</v>
+      </c>
+      <c r="D13" s="4" t="s">
+        <v>112</v>
+      </c>
+      <c r="E13" s="3" t="s">
+        <v>90</v>
+      </c>
+      <c r="F13" s="5" t="s">
+        <v>113</v>
+      </c>
+      <c r="G13" s="5" t="s">
+        <v>113</v>
+      </c>
+      <c r="H13" s="6" t="s">
+        <v>121</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" scale="51" orientation="landscape" verticalDpi="300" r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:H12"/>
+  <sheetViews>
+    <sheetView topLeftCell="B1" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
+      <selection activeCell="K5" sqref="K5"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="13.140625" customWidth="1"/>
+    <col min="2" max="2" width="42.140625" customWidth="1"/>
+    <col min="3" max="3" width="30" customWidth="1"/>
+    <col min="4" max="4" width="38.42578125" customWidth="1"/>
+    <col min="5" max="5" width="11.7109375" customWidth="1"/>
+    <col min="6" max="6" width="47.28515625" customWidth="1"/>
+    <col min="7" max="7" width="49.140625" customWidth="1"/>
+    <col min="8" max="8" width="26.42578125" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:8" ht="51" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A1" s="2" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" s="2" t="s">
+        <v>88</v>
+      </c>
+      <c r="D1" s="2" t="s">
+        <v>2</v>
+      </c>
+      <c r="E1" s="2" t="s">
+        <v>3</v>
+      </c>
+      <c r="F1" s="2" t="s">
+        <v>4</v>
+      </c>
+      <c r="G1" s="2" t="s">
+        <v>5</v>
+      </c>
+      <c r="H1" s="2" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="2" spans="1:8" ht="60" x14ac:dyDescent="0.25">
+      <c r="A2" s="3" t="s">
+        <v>15</v>
+      </c>
+      <c r="B2" s="5" t="s">
+        <v>54</v>
+      </c>
+      <c r="C2" s="3" t="s">
+        <v>90</v>
+      </c>
+      <c r="D2" s="4" t="s">
+        <v>52</v>
+      </c>
+      <c r="E2" s="3" t="s">
+        <v>90</v>
+      </c>
+      <c r="F2" s="5" t="s">
+        <v>53</v>
+      </c>
+      <c r="G2" s="5" t="s">
+        <v>122</v>
+      </c>
+      <c r="H2" s="6" t="s">
+        <v>121</v>
+      </c>
+    </row>
+    <row r="3" spans="1:8" ht="45" x14ac:dyDescent="0.25">
+      <c r="A3" s="3" t="s">
+        <v>18</v>
+      </c>
+      <c r="B3" s="3" t="s">
+        <v>60</v>
+      </c>
+      <c r="C3" s="3" t="s">
+        <v>90</v>
+      </c>
+      <c r="D3" s="4" t="s">
+        <v>61</v>
+      </c>
+      <c r="E3" s="3" t="s">
+        <v>90</v>
+      </c>
+      <c r="F3" s="5" t="s">
+        <v>62</v>
+      </c>
+      <c r="G3" s="5" t="s">
+        <v>62</v>
+      </c>
+      <c r="H3" s="6" t="s">
+        <v>121</v>
+      </c>
+    </row>
+    <row r="4" spans="1:8" ht="60" x14ac:dyDescent="0.25">
+      <c r="A4" s="3" t="s">
+        <v>19</v>
+      </c>
+      <c r="B4" s="3" t="s">
+        <v>63</v>
+      </c>
+      <c r="C4" s="3" t="s">
+        <v>90</v>
+      </c>
+      <c r="D4" s="4" t="s">
+        <v>64</v>
+      </c>
+      <c r="E4" s="3" t="s">
+        <v>90</v>
+      </c>
+      <c r="F4" s="5" t="s">
+        <v>65</v>
+      </c>
+      <c r="G4" s="3" t="s">
+        <v>124</v>
+      </c>
+      <c r="H4" s="8" t="s">
+        <v>123</v>
+      </c>
+    </row>
+    <row r="5" spans="1:8" ht="60" x14ac:dyDescent="0.25">
+      <c r="A5" s="3" t="s">
+        <v>20</v>
+      </c>
+      <c r="B5" s="5" t="s">
+        <v>66</v>
+      </c>
+      <c r="C5" s="3" t="s">
+        <v>90</v>
+      </c>
+      <c r="D5" s="4" t="s">
+        <v>33</v>
+      </c>
+      <c r="E5" s="3" t="s">
+        <v>90</v>
+      </c>
+      <c r="F5" s="5" t="s">
+        <v>67</v>
+      </c>
+      <c r="G5" s="5" t="s">
+        <v>125</v>
+      </c>
+      <c r="H5" s="8" t="s">
+        <v>123</v>
+      </c>
+    </row>
+    <row r="6" spans="1:8" ht="60" x14ac:dyDescent="0.25">
+      <c r="A6" s="3" t="s">
+        <v>24</v>
+      </c>
+      <c r="B6" s="5" t="s">
+        <v>72</v>
+      </c>
+      <c r="C6" s="5" t="s">
+        <v>91</v>
+      </c>
+      <c r="D6" s="4" t="s">
+        <v>74</v>
+      </c>
+      <c r="E6" s="3" t="s">
+        <v>90</v>
+      </c>
+      <c r="F6" s="5" t="s">
+        <v>79</v>
+      </c>
+      <c r="G6" s="3" t="s">
+        <v>126</v>
+      </c>
+      <c r="H6" s="6" t="s">
+        <v>121</v>
+      </c>
+    </row>
+    <row r="7" spans="1:8" ht="60" x14ac:dyDescent="0.25">
+      <c r="A7" s="3" t="s">
+        <v>25</v>
+      </c>
+      <c r="B7" s="5" t="s">
+        <v>73</v>
+      </c>
+      <c r="C7" s="3" t="s">
+        <v>90</v>
+      </c>
+      <c r="D7" s="4" t="s">
+        <v>75</v>
+      </c>
+      <c r="E7" s="3" t="s">
+        <v>90</v>
+      </c>
+      <c r="F7" s="5" t="s">
+        <v>78</v>
+      </c>
+      <c r="G7" s="5" t="s">
+        <v>78</v>
+      </c>
+      <c r="H7" s="6" t="s">
+        <v>121</v>
+      </c>
+    </row>
+    <row r="8" spans="1:8" ht="75" x14ac:dyDescent="0.25">
+      <c r="A8" s="3" t="s">
+        <v>28</v>
+      </c>
+      <c r="B8" s="5" t="s">
+        <v>85</v>
+      </c>
+      <c r="C8" s="3" t="s">
+        <v>90</v>
+      </c>
+      <c r="D8" s="4" t="s">
+        <v>84</v>
+      </c>
+      <c r="E8" s="3" t="s">
+        <v>90</v>
+      </c>
+      <c r="F8" s="5" t="s">
+        <v>87</v>
+      </c>
+      <c r="G8" s="5" t="s">
+        <v>87</v>
+      </c>
+      <c r="H8" s="6" t="s">
+        <v>121</v>
+      </c>
+    </row>
+    <row r="9" spans="1:8" ht="60" x14ac:dyDescent="0.25">
+      <c r="A9" s="3" t="s">
+        <v>29</v>
+      </c>
+      <c r="B9" s="5" t="s">
+        <v>86</v>
+      </c>
+      <c r="C9" s="3" t="s">
+        <v>90</v>
+      </c>
+      <c r="D9" s="4" t="s">
+        <v>75</v>
+      </c>
+      <c r="E9" s="3" t="s">
+        <v>90</v>
+      </c>
+      <c r="F9" s="5" t="s">
+        <v>87</v>
+      </c>
+      <c r="G9" s="5" t="s">
+        <v>87</v>
+      </c>
+      <c r="H9" s="6" t="s">
+        <v>121</v>
+      </c>
+    </row>
+    <row r="10" spans="1:8" ht="45" x14ac:dyDescent="0.25">
+      <c r="A10" s="3" t="s">
+        <v>117</v>
+      </c>
+      <c r="B10" s="5" t="s">
+        <v>102</v>
+      </c>
+      <c r="C10" s="3" t="s">
+        <v>90</v>
+      </c>
+      <c r="D10" s="4" t="s">
+        <v>103</v>
+      </c>
+      <c r="E10" s="3" t="s">
+        <v>90</v>
+      </c>
+      <c r="F10" s="5" t="s">
+        <v>104</v>
+      </c>
+      <c r="G10" s="5" t="s">
+        <v>104</v>
+      </c>
+      <c r="H10" s="6" t="s">
+        <v>121</v>
+      </c>
+    </row>
+    <row r="11" spans="1:8" ht="105" x14ac:dyDescent="0.25">
+      <c r="A11" s="3" t="s">
+        <v>118</v>
+      </c>
+      <c r="B11" s="5" t="s">
+        <v>105</v>
+      </c>
+      <c r="C11" s="3" t="s">
+        <v>90</v>
+      </c>
+      <c r="D11" s="4" t="s">
+        <v>106</v>
+      </c>
+      <c r="E11" s="3" t="s">
+        <v>90</v>
+      </c>
+      <c r="F11" s="5" t="s">
+        <v>107</v>
+      </c>
+      <c r="G11" s="5" t="s">
+        <v>107</v>
+      </c>
+      <c r="H11" s="6" t="s">
+        <v>121</v>
+      </c>
+    </row>
+    <row r="12" spans="1:8" ht="165" x14ac:dyDescent="0.25">
+      <c r="A12" s="3" t="s">
+        <v>119</v>
+      </c>
+      <c r="B12" s="5" t="s">
+        <v>108</v>
+      </c>
+      <c r="C12" s="5" t="s">
+        <v>89</v>
+      </c>
+      <c r="D12" s="4" t="s">
+        <v>109</v>
+      </c>
+      <c r="E12" s="3" t="s">
+        <v>90</v>
+      </c>
+      <c r="F12" s="5" t="s">
+        <v>110</v>
+      </c>
+      <c r="G12" s="5" t="s">
+        <v>110</v>
+      </c>
+      <c r="H12" s="6" t="s">
+        <v>121</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" scale="51" orientation="landscape" verticalDpi="300" r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:H38"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="B4" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <selection activeCell="C6" sqref="C6"/>
+    <sheetView zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
+      <selection activeCell="K2" sqref="K2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>

</xml_diff>